<commit_message>
feat: finalize home impl reports
</commit_message>
<xml_diff>
--- a/examples/financial-report.xlsx
+++ b/examples/financial-report.xlsx
@@ -32,8 +32,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <numFmts count="11">
-    <numFmt numFmtId="165" formatCode="mmm yyyy"/>
+  <numFmts count="12">
+    <numFmt numFmtId="165" formatCode="MMM YYYY"/>
     <numFmt numFmtId="166" formatCode="$#,##0.00"/>
     <numFmt numFmtId="167" formatCode="$#,##0.00"/>
     <numFmt numFmtId="168" formatCode="$#,##0.00"/>
@@ -44,8 +44,9 @@
     <numFmt numFmtId="173" formatCode="$#,##0.00"/>
     <numFmt numFmtId="174" formatCode="$#,##0.00"/>
     <numFmt numFmtId="175" formatCode="$#,##0.00"/>
+    <numFmt numFmtId="176" formatCode="$#,##0.00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -87,12 +88,27 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <color rgb="FF0000"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <color rgb="FF0000"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <color rgb="007500"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <color rgb="007500"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <color rgb="FF0000"/>
     </font>
     <font>
       <sz val="11"/>
@@ -168,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -535,6 +551,51 @@
       <right style="thin">
         <color rgb="000000"/>
       </right>
+      <top style="medium">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="000000"/>
+      </right>
       <top style="thin">
         <color rgb="000000"/>
       </top>
@@ -577,7 +638,7 @@
   <cellStyleXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -650,13 +711,22 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="14" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="16" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="17" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="18" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1042,34 +1112,34 @@
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="4" t="str">
-        <v>2023-06</v>
+        <v>2023-11</v>
       </c>
       <c r="B2" s="5" t="str">
-        <v>Marketing</v>
+        <v>Human Resources</v>
       </c>
       <c r="C2" s="6">
-        <v>38705</v>
+        <v>81062</v>
       </c>
       <c r="D2" s="6">
-        <v>8841</v>
+        <v>9353</v>
       </c>
       <c r="E2" s="7">
-        <v>29864</v>
+        <v>71709</v>
       </c>
       <c r="F2" s="8" t="str">
-        <v>77.16%</v>
+        <v>88.46%</v>
       </c>
       <c r="G2" s="6">
-        <v>170049</v>
+        <v>190569</v>
       </c>
       <c r="H2" s="6">
-        <v>56008</v>
+        <v>65402</v>
       </c>
       <c r="I2" s="7">
-        <v>114041</v>
+        <v>125167</v>
       </c>
       <c r="J2" s="9">
-        <v>66.74</v>
+        <v>32.88</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
@@ -1077,19 +1147,19 @@
         <v/>
       </c>
       <c r="B3" s="11" t="str">
-        <v>Human Resources</v>
+        <v>Customer Support</v>
       </c>
       <c r="C3" s="12">
-        <v>83780</v>
+        <v>82566</v>
       </c>
       <c r="D3" s="12">
-        <v>24449</v>
+        <v>7289</v>
       </c>
       <c r="E3" s="13">
-        <v>59331</v>
+        <v>75277</v>
       </c>
       <c r="F3" s="14" t="str">
-        <v>70.82%</v>
+        <v>91.17%</v>
       </c>
       <c r="G3" s="11" t="str">
         <v/>
@@ -1109,19 +1179,19 @@
         <v/>
       </c>
       <c r="B4" s="17" t="str">
-        <v>Marketing</v>
+        <v>Customer Support</v>
       </c>
       <c r="C4" s="18">
-        <v>47564</v>
+        <v>26941</v>
       </c>
       <c r="D4" s="18">
-        <v>22718</v>
+        <v>48760</v>
       </c>
       <c r="E4" s="19">
-        <v>24846</v>
+        <v>-21819</v>
       </c>
       <c r="F4" s="20" t="str">
-        <v>52.24%</v>
+        <v>-80.99%</v>
       </c>
       <c r="G4" s="17" t="str">
         <v/>
@@ -1138,34 +1208,34 @@
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="4" t="str">
-        <v>2023-08</v>
+        <v>2023-04</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Marketing</v>
+        <v>Sales</v>
       </c>
       <c r="C5" s="6">
-        <v>54644</v>
+        <v>94554</v>
       </c>
       <c r="D5" s="6">
-        <v>26682</v>
+        <v>8208</v>
       </c>
       <c r="E5" s="7">
-        <v>27962</v>
+        <v>86346</v>
       </c>
       <c r="F5" s="8" t="str">
-        <v>51.17%</v>
+        <v>91.32%</v>
       </c>
       <c r="G5" s="6">
-        <v>225676</v>
+        <v>131885</v>
       </c>
       <c r="H5" s="6">
-        <v>103143</v>
+        <v>41402</v>
       </c>
       <c r="I5" s="7">
-        <v>122533</v>
+        <v>90483</v>
       </c>
       <c r="J5" s="9">
-        <v>54.42666666666667</v>
+        <v>27.869999999999994</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
@@ -1173,19 +1243,19 @@
         <v/>
       </c>
       <c r="B6" s="11" t="str">
-        <v>Customer Support</v>
+        <v>Human Resources</v>
       </c>
       <c r="C6" s="12">
-        <v>78442</v>
+        <v>22132</v>
       </c>
       <c r="D6" s="12">
-        <v>27233</v>
+        <v>5186</v>
       </c>
       <c r="E6" s="13">
-        <v>51209</v>
+        <v>16946</v>
       </c>
       <c r="F6" s="14" t="str">
-        <v>65.28%</v>
+        <v>76.57%</v>
       </c>
       <c r="G6" s="11" t="str">
         <v/>
@@ -1208,16 +1278,16 @@
         <v>Marketing</v>
       </c>
       <c r="C7" s="18">
-        <v>92590</v>
+        <v>15199</v>
       </c>
       <c r="D7" s="18">
-        <v>49228</v>
+        <v>28008</v>
       </c>
       <c r="E7" s="19">
-        <v>43362</v>
+        <v>-12809</v>
       </c>
       <c r="F7" s="20" t="str">
-        <v>46.83%</v>
+        <v>-84.28%</v>
       </c>
       <c r="G7" s="17" t="str">
         <v/>
@@ -1234,34 +1304,34 @@
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="str">
-        <v>2023-03</v>
+        <v>2023-08</v>
       </c>
       <c r="B8" s="5" t="str">
         <v>R&amp;D</v>
       </c>
       <c r="C8" s="6">
-        <v>89616</v>
+        <v>44553</v>
       </c>
       <c r="D8" s="6">
-        <v>23948</v>
+        <v>26637</v>
       </c>
       <c r="E8" s="7">
-        <v>65668</v>
+        <v>17916</v>
       </c>
       <c r="F8" s="8" t="str">
-        <v>73.28%</v>
+        <v>40.21%</v>
       </c>
       <c r="G8" s="6">
-        <v>179457</v>
+        <v>143950</v>
       </c>
       <c r="H8" s="6">
-        <v>39671</v>
+        <v>68048</v>
       </c>
       <c r="I8" s="7">
-        <v>139786</v>
+        <v>75902</v>
       </c>
       <c r="J8" s="9">
-        <v>70.56333333333333</v>
+        <v>31.166666666666668</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
@@ -1272,16 +1342,16 @@
         <v>Marketing</v>
       </c>
       <c r="C9" s="12">
-        <v>78258</v>
+        <v>78755</v>
       </c>
       <c r="D9" s="12">
-        <v>10081</v>
+        <v>15077</v>
       </c>
       <c r="E9" s="13">
-        <v>68177</v>
+        <v>63678</v>
       </c>
       <c r="F9" s="14" t="str">
-        <v>87.12%</v>
+        <v>80.86%</v>
       </c>
       <c r="G9" s="11" t="str">
         <v/>
@@ -1301,19 +1371,19 @@
         <v/>
       </c>
       <c r="B10" s="17" t="str">
-        <v>Human Resources</v>
+        <v>Marketing</v>
       </c>
       <c r="C10" s="18">
-        <v>11583</v>
+        <v>20642</v>
       </c>
       <c r="D10" s="18">
-        <v>5642</v>
+        <v>26334</v>
       </c>
       <c r="E10" s="19">
-        <v>5941</v>
+        <v>-5692</v>
       </c>
       <c r="F10" s="20" t="str">
-        <v>51.29%</v>
+        <v>-27.57%</v>
       </c>
       <c r="G10" s="17" t="str">
         <v/>
@@ -1330,34 +1400,34 @@
     </row>
     <row r="11" ht="30" customHeight="1">
       <c r="A11" s="4" t="str">
-        <v>2023-01</v>
+        <v>2023-02</v>
       </c>
       <c r="B11" s="5" t="str">
         <v>Human Resources</v>
       </c>
       <c r="C11" s="6">
-        <v>71261</v>
+        <v>14471</v>
       </c>
       <c r="D11" s="6">
-        <v>47935</v>
+        <v>12779</v>
       </c>
       <c r="E11" s="7">
-        <v>23326</v>
+        <v>1692</v>
       </c>
       <c r="F11" s="8" t="str">
-        <v>32.73%</v>
+        <v>11.69%</v>
       </c>
       <c r="G11" s="6">
-        <v>229711</v>
+        <v>108693</v>
       </c>
       <c r="H11" s="6">
-        <v>142357</v>
+        <v>83003</v>
       </c>
       <c r="I11" s="7">
-        <v>87354</v>
+        <v>25690</v>
       </c>
       <c r="J11" s="9">
-        <v>35.69333333333333</v>
+        <v>21.576666666666668</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
@@ -1368,16 +1438,16 @@
         <v>Marketing</v>
       </c>
       <c r="C12" s="12">
-        <v>95231</v>
+        <v>38750</v>
       </c>
       <c r="D12" s="12">
-        <v>44581</v>
+        <v>26175</v>
       </c>
       <c r="E12" s="13">
-        <v>50650</v>
+        <v>12575</v>
       </c>
       <c r="F12" s="14" t="str">
-        <v>53.19%</v>
+        <v>32.45%</v>
       </c>
       <c r="G12" s="11" t="str">
         <v/>
@@ -1397,19 +1467,19 @@
         <v/>
       </c>
       <c r="B13" s="17" t="str">
-        <v>R&amp;D</v>
+        <v>Human Resources</v>
       </c>
       <c r="C13" s="18">
-        <v>63219</v>
+        <v>55472</v>
       </c>
       <c r="D13" s="18">
-        <v>49841</v>
-      </c>
-      <c r="E13" s="19">
-        <v>13378</v>
-      </c>
-      <c r="F13" s="20" t="str">
-        <v>21.16%</v>
+        <v>44049</v>
+      </c>
+      <c r="E13" s="22">
+        <v>11423</v>
+      </c>
+      <c r="F13" s="23" t="str">
+        <v>20.59%</v>
       </c>
       <c r="G13" s="17" t="str">
         <v/>
@@ -1426,34 +1496,34 @@
     </row>
     <row r="14" ht="30" customHeight="1">
       <c r="A14" s="4" t="str">
-        <v>2023-04</v>
+        <v>2023-12</v>
       </c>
       <c r="B14" s="5" t="str">
         <v>Sales</v>
       </c>
       <c r="C14" s="6">
-        <v>72650</v>
+        <v>63665</v>
       </c>
       <c r="D14" s="6">
-        <v>14333</v>
+        <v>13875</v>
       </c>
       <c r="E14" s="7">
-        <v>58317</v>
+        <v>49790</v>
       </c>
       <c r="F14" s="8" t="str">
-        <v>80.27%</v>
+        <v>78.21%</v>
       </c>
       <c r="G14" s="6">
-        <v>172699</v>
+        <v>179351</v>
       </c>
       <c r="H14" s="6">
-        <v>64105</v>
+        <v>98130</v>
       </c>
       <c r="I14" s="7">
-        <v>108594</v>
+        <v>81221</v>
       </c>
       <c r="J14" s="9">
-        <v>57.82999999999999</v>
+        <v>5.143333333333331</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
@@ -1464,16 +1534,16 @@
         <v>Human Resources</v>
       </c>
       <c r="C15" s="12">
-        <v>55182</v>
+        <v>18683</v>
       </c>
       <c r="D15" s="12">
-        <v>9970</v>
-      </c>
-      <c r="E15" s="13">
-        <v>45212</v>
-      </c>
-      <c r="F15" s="14" t="str">
-        <v>81.93%</v>
+        <v>40709</v>
+      </c>
+      <c r="E15" s="24">
+        <v>-22026</v>
+      </c>
+      <c r="F15" s="25" t="str">
+        <v>-117.89%</v>
       </c>
       <c r="G15" s="11" t="str">
         <v/>
@@ -1496,16 +1566,16 @@
         <v>Customer Support</v>
       </c>
       <c r="C16" s="18">
-        <v>44867</v>
+        <v>97003</v>
       </c>
       <c r="D16" s="18">
-        <v>39802</v>
-      </c>
-      <c r="E16" s="19">
-        <v>5065</v>
-      </c>
-      <c r="F16" s="20" t="str">
-        <v>11.29%</v>
+        <v>43546</v>
+      </c>
+      <c r="E16" s="22">
+        <v>53457</v>
+      </c>
+      <c r="F16" s="23" t="str">
+        <v>55.11%</v>
       </c>
       <c r="G16" s="17" t="str">
         <v/>
@@ -1522,34 +1592,34 @@
     </row>
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="4" t="str">
-        <v>2023-12</v>
+        <v>2023-11</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>R&amp;D</v>
+        <v>Customer Support</v>
       </c>
       <c r="C17" s="6">
-        <v>83844</v>
+        <v>40686</v>
       </c>
       <c r="D17" s="6">
-        <v>31484</v>
+        <v>15065</v>
       </c>
       <c r="E17" s="7">
-        <v>52360</v>
+        <v>25621</v>
       </c>
       <c r="F17" s="8" t="str">
-        <v>62.45%</v>
+        <v>62.97%</v>
       </c>
       <c r="G17" s="6">
-        <v>241972</v>
+        <v>150765</v>
       </c>
       <c r="H17" s="6">
-        <v>93768</v>
+        <v>49381</v>
       </c>
       <c r="I17" s="7">
-        <v>148204</v>
+        <v>101384</v>
       </c>
       <c r="J17" s="9">
-        <v>60.81</v>
+        <v>67.19666666666666</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
@@ -1557,19 +1627,19 @@
         <v/>
       </c>
       <c r="B18" s="11" t="str">
-        <v>Human Resources</v>
+        <v>Marketing</v>
       </c>
       <c r="C18" s="12">
-        <v>76752</v>
+        <v>65011</v>
       </c>
       <c r="D18" s="12">
-        <v>46978</v>
+        <v>21693</v>
       </c>
       <c r="E18" s="13">
-        <v>29774</v>
+        <v>43318</v>
       </c>
       <c r="F18" s="14" t="str">
-        <v>38.79%</v>
+        <v>66.63%</v>
       </c>
       <c r="G18" s="11" t="str">
         <v/>
@@ -1592,16 +1662,16 @@
         <v>Sales</v>
       </c>
       <c r="C19" s="18">
-        <v>81376</v>
+        <v>45068</v>
       </c>
       <c r="D19" s="18">
-        <v>15306</v>
-      </c>
-      <c r="E19" s="19">
-        <v>66070</v>
-      </c>
-      <c r="F19" s="20" t="str">
-        <v>81.19%</v>
+        <v>12623</v>
+      </c>
+      <c r="E19" s="22">
+        <v>32445</v>
+      </c>
+      <c r="F19" s="23" t="str">
+        <v>71.99%</v>
       </c>
       <c r="G19" s="17" t="str">
         <v/>
@@ -1621,31 +1691,31 @@
         <v>2023-09</v>
       </c>
       <c r="B20" s="5" t="str">
-        <v>R&amp;D</v>
+        <v>Human Resources</v>
       </c>
       <c r="C20" s="6">
-        <v>74493</v>
+        <v>93311</v>
       </c>
       <c r="D20" s="6">
-        <v>14817</v>
+        <v>34997</v>
       </c>
       <c r="E20" s="7">
-        <v>59676</v>
+        <v>58314</v>
       </c>
       <c r="F20" s="8" t="str">
-        <v>80.11%</v>
+        <v>62.49%</v>
       </c>
       <c r="G20" s="6">
-        <v>136882</v>
+        <v>207856</v>
       </c>
       <c r="H20" s="6">
-        <v>64428</v>
+        <v>99527</v>
       </c>
       <c r="I20" s="7">
-        <v>72454</v>
+        <v>108329</v>
       </c>
       <c r="J20" s="9">
-        <v>33.89333333333334</v>
+        <v>39.39666666666667</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
@@ -1653,19 +1723,19 @@
         <v/>
       </c>
       <c r="B21" s="11" t="str">
-        <v>Sales</v>
+        <v>Human Resources</v>
       </c>
       <c r="C21" s="12">
-        <v>43913</v>
+        <v>78484</v>
       </c>
       <c r="D21" s="12">
-        <v>28735</v>
+        <v>23113</v>
       </c>
       <c r="E21" s="13">
-        <v>15178</v>
+        <v>55371</v>
       </c>
       <c r="F21" s="14" t="str">
-        <v>34.56%</v>
+        <v>70.55%</v>
       </c>
       <c r="G21" s="11" t="str">
         <v/>
@@ -1688,16 +1758,16 @@
         <v>R&amp;D</v>
       </c>
       <c r="C22" s="18">
-        <v>18476</v>
+        <v>36061</v>
       </c>
       <c r="D22" s="18">
-        <v>20876</v>
-      </c>
-      <c r="E22" s="22">
-        <v>-2400</v>
-      </c>
-      <c r="F22" s="23" t="str">
-        <v>-12.99%</v>
+        <v>41417</v>
+      </c>
+      <c r="E22" s="19">
+        <v>-5356</v>
+      </c>
+      <c r="F22" s="20" t="str">
+        <v>-14.85%</v>
       </c>
       <c r="G22" s="17" t="str">
         <v/>
@@ -1714,34 +1784,34 @@
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="4" t="str">
-        <v>2023-11</v>
+        <v>2023-03</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>Marketing</v>
+        <v>Human Resources</v>
       </c>
       <c r="C23" s="6">
-        <v>11657</v>
+        <v>21324</v>
       </c>
       <c r="D23" s="6">
-        <v>5269</v>
-      </c>
-      <c r="E23" s="7">
-        <v>6388</v>
-      </c>
-      <c r="F23" s="8" t="str">
-        <v>54.8%</v>
+        <v>29992</v>
+      </c>
+      <c r="E23" s="26">
+        <v>-8668</v>
+      </c>
+      <c r="F23" s="27" t="str">
+        <v>-40.65%</v>
       </c>
       <c r="G23" s="6">
-        <v>130398</v>
+        <v>178802</v>
       </c>
       <c r="H23" s="6">
-        <v>60361</v>
+        <v>85762</v>
       </c>
       <c r="I23" s="7">
-        <v>70037</v>
+        <v>93040</v>
       </c>
       <c r="J23" s="9">
-        <v>59.093333333333334</v>
+        <v>29.566666666666674</v>
       </c>
     </row>
     <row r="24" ht="30" customHeight="1">
@@ -1752,16 +1822,16 @@
         <v>Marketing</v>
       </c>
       <c r="C24" s="12">
-        <v>32330</v>
+        <v>66369</v>
       </c>
       <c r="D24" s="12">
-        <v>7113</v>
+        <v>23057</v>
       </c>
       <c r="E24" s="13">
-        <v>25217</v>
+        <v>43312</v>
       </c>
       <c r="F24" s="14" t="str">
-        <v>78%</v>
+        <v>65.26%</v>
       </c>
       <c r="G24" s="11" t="str">
         <v/>
@@ -1781,19 +1851,19 @@
         <v/>
       </c>
       <c r="B25" s="17" t="str">
-        <v>R&amp;D</v>
+        <v>Marketing</v>
       </c>
       <c r="C25" s="18">
-        <v>86411</v>
+        <v>91109</v>
       </c>
       <c r="D25" s="18">
-        <v>47979</v>
-      </c>
-      <c r="E25" s="19">
-        <v>38432</v>
-      </c>
-      <c r="F25" s="20" t="str">
-        <v>44.48%</v>
+        <v>32713</v>
+      </c>
+      <c r="E25" s="22">
+        <v>58396</v>
+      </c>
+      <c r="F25" s="23" t="str">
+        <v>64.09%</v>
       </c>
       <c r="G25" s="17" t="str">
         <v/>
@@ -1810,34 +1880,34 @@
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="A26" s="4" t="str">
-        <v>2023-05</v>
+        <v>2023-09</v>
       </c>
       <c r="B26" s="5" t="str">
-        <v>Marketing</v>
+        <v>Human Resources</v>
       </c>
       <c r="C26" s="6">
-        <v>80369</v>
+        <v>30229</v>
       </c>
       <c r="D26" s="6">
-        <v>22211</v>
-      </c>
-      <c r="E26" s="7">
-        <v>58158</v>
-      </c>
-      <c r="F26" s="8" t="str">
-        <v>72.36%</v>
+        <v>45548</v>
+      </c>
+      <c r="E26" s="26">
+        <v>-15319</v>
+      </c>
+      <c r="F26" s="27" t="str">
+        <v>-50.68%</v>
       </c>
       <c r="G26" s="6">
-        <v>200863</v>
+        <v>96893</v>
       </c>
       <c r="H26" s="6">
-        <v>75267</v>
+        <v>83467</v>
       </c>
       <c r="I26" s="7">
-        <v>125596</v>
+        <v>13426</v>
       </c>
       <c r="J26" s="9">
-        <v>49.49666666666667</v>
+        <v>6.23</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1">
@@ -1848,16 +1918,16 @@
         <v>Customer Support</v>
       </c>
       <c r="C27" s="12">
-        <v>34227</v>
+        <v>42373</v>
       </c>
       <c r="D27" s="12">
-        <v>35387</v>
-      </c>
-      <c r="E27" s="24">
-        <v>-1160</v>
-      </c>
-      <c r="F27" s="25" t="str">
-        <v>-3.39%</v>
+        <v>14500</v>
+      </c>
+      <c r="E27" s="13">
+        <v>27873</v>
+      </c>
+      <c r="F27" s="14" t="str">
+        <v>65.78%</v>
       </c>
       <c r="G27" s="11" t="str">
         <v/>
@@ -1877,19 +1947,19 @@
         <v/>
       </c>
       <c r="B28" s="17" t="str">
-        <v>Customer Support</v>
+        <v>Marketing</v>
       </c>
       <c r="C28" s="18">
-        <v>86267</v>
+        <v>24291</v>
       </c>
       <c r="D28" s="18">
-        <v>17669</v>
-      </c>
-      <c r="E28" s="19">
-        <v>68598</v>
-      </c>
-      <c r="F28" s="20" t="str">
-        <v>79.52%</v>
+        <v>23419</v>
+      </c>
+      <c r="E28" s="22">
+        <v>872</v>
+      </c>
+      <c r="F28" s="23" t="str">
+        <v>3.59%</v>
       </c>
       <c r="G28" s="17" t="str">
         <v/>
@@ -1906,34 +1976,34 @@
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" s="4" t="str">
-        <v>2023-10</v>
+        <v>2023-11</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>Customer Support</v>
+        <v>Human Resources</v>
       </c>
       <c r="C29" s="6">
-        <v>55453</v>
+        <v>25344</v>
       </c>
       <c r="D29" s="6">
-        <v>38557</v>
-      </c>
-      <c r="E29" s="7">
-        <v>16896</v>
-      </c>
-      <c r="F29" s="8" t="str">
-        <v>30.47%</v>
+        <v>36441</v>
+      </c>
+      <c r="E29" s="26">
+        <v>-11097</v>
+      </c>
+      <c r="F29" s="27" t="str">
+        <v>-43.79%</v>
       </c>
       <c r="G29" s="6">
-        <v>161623</v>
+        <v>98040</v>
       </c>
       <c r="H29" s="6">
-        <v>102111</v>
+        <v>80362</v>
       </c>
       <c r="I29" s="7">
-        <v>59512</v>
-      </c>
-      <c r="J29" s="9">
-        <v>15.599999999999996</v>
+        <v>17678</v>
+      </c>
+      <c r="J29" s="28">
+        <v>-4.073333333333335</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1">
@@ -1941,19 +2011,19 @@
         <v/>
       </c>
       <c r="B30" s="11" t="str">
-        <v>Customer Support</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C30" s="12">
-        <v>76725</v>
+        <v>51884</v>
       </c>
       <c r="D30" s="12">
-        <v>15374</v>
+        <v>14807</v>
       </c>
       <c r="E30" s="13">
-        <v>61351</v>
+        <v>37077</v>
       </c>
       <c r="F30" s="14" t="str">
-        <v>79.96%</v>
+        <v>71.46%</v>
       </c>
       <c r="G30" s="11" t="str">
         <v/>
@@ -1973,19 +2043,19 @@
         <v/>
       </c>
       <c r="B31" s="17" t="str">
-        <v>Marketing</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C31" s="18">
-        <v>29445</v>
+        <v>20812</v>
       </c>
       <c r="D31" s="18">
-        <v>48180</v>
-      </c>
-      <c r="E31" s="22">
-        <v>-18735</v>
-      </c>
-      <c r="F31" s="23" t="str">
-        <v>-63.63%</v>
+        <v>29114</v>
+      </c>
+      <c r="E31" s="19">
+        <v>-8302</v>
+      </c>
+      <c r="F31" s="20" t="str">
+        <v>-39.89%</v>
       </c>
       <c r="G31" s="17" t="str">
         <v/>
@@ -2001,17 +2071,17 @@
       </c>
     </row>
     <row r="32" ht="30" customHeight="1">
-      <c r="G32" s="26">
-        <v>1849330</v>
-      </c>
-      <c r="H32" s="26">
-        <v>801219</v>
-      </c>
-      <c r="I32" s="27">
-        <v>1048111</v>
-      </c>
-      <c r="J32" s="28">
-        <v>50.41466666666666</v>
+      <c r="G32" s="29">
+        <v>1486804</v>
+      </c>
+      <c r="H32" s="29">
+        <v>754484</v>
+      </c>
+      <c r="I32" s="30">
+        <v>732320</v>
+      </c>
+      <c r="J32" s="31">
+        <v>25.69533333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add column header styling support
</commit_message>
<xml_diff>
--- a/examples/financial-report.xlsx
+++ b/examples/financial-report.xlsx
@@ -88,7 +88,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <color rgb="007500"/>
+      <color rgb="FF0000"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <color rgb="FF0000"/>
     </font>
     <font>
       <sz val="11"/>
@@ -98,12 +103,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <color rgb="FF0000"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <color rgb="FF0000"/>
+      <color rgb="007500"/>
     </font>
     <font>
       <sz val="11"/>
@@ -491,6 +491,36 @@
       <right style="thin">
         <color rgb="000000"/>
       </right>
+      <top style="thin">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="000000"/>
+      </right>
       <top style="medium">
         <color rgb="000000"/>
       </top>
@@ -555,36 +585,6 @@
         <color rgb="000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000"/>
-      </top>
-      <bottom style="medium">
         <color rgb="000000"/>
       </bottom>
       <diagonal/>
@@ -705,13 +705,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="174" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
@@ -1112,34 +1112,34 @@
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="4" t="str">
-        <v>2023-10</v>
+        <v>2023-05</v>
       </c>
       <c r="B2" s="5" t="str">
-        <v>Customer Support</v>
+        <v>Marketing</v>
       </c>
       <c r="C2" s="6">
-        <v>38540</v>
+        <v>84367</v>
       </c>
       <c r="D2" s="6">
-        <v>8257</v>
+        <v>38132</v>
       </c>
       <c r="E2" s="7">
-        <v>30283</v>
+        <v>46235</v>
       </c>
       <c r="F2" s="8" t="str">
-        <v>78.58%</v>
+        <v>54.8%</v>
       </c>
       <c r="G2" s="6">
-        <v>172133</v>
+        <v>218543</v>
       </c>
       <c r="H2" s="6">
-        <v>54770</v>
+        <v>120412</v>
       </c>
       <c r="I2" s="7">
-        <v>117363</v>
+        <v>98131</v>
       </c>
       <c r="J2" s="9">
-        <v>69.23</v>
+        <v>33.78666666666667</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
@@ -1150,16 +1150,16 @@
         <v>Marketing</v>
       </c>
       <c r="C3" s="12">
-        <v>78403</v>
+        <v>93734</v>
       </c>
       <c r="D3" s="12">
-        <v>24962</v>
+        <v>35578</v>
       </c>
       <c r="E3" s="13">
-        <v>53441</v>
+        <v>58156</v>
       </c>
       <c r="F3" s="14" t="str">
-        <v>68.16%</v>
+        <v>62.04%</v>
       </c>
       <c r="G3" s="11" t="str">
         <v/>
@@ -1179,19 +1179,19 @@
         <v/>
       </c>
       <c r="B4" s="17" t="str">
-        <v>Human Resources</v>
+        <v>Marketing</v>
       </c>
       <c r="C4" s="18">
-        <v>55190</v>
+        <v>40442</v>
       </c>
       <c r="D4" s="18">
-        <v>21551</v>
+        <v>46702</v>
       </c>
       <c r="E4" s="19">
-        <v>33639</v>
+        <v>-6260</v>
       </c>
       <c r="F4" s="20" t="str">
-        <v>60.95%</v>
+        <v>-15.48%</v>
       </c>
       <c r="G4" s="17" t="str">
         <v/>
@@ -1208,34 +1208,34 @@
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="4" t="str">
-        <v>2023-04</v>
+        <v>2023-07</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Marketing</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C5" s="6">
-        <v>85863</v>
+        <v>94769</v>
       </c>
       <c r="D5" s="6">
-        <v>14549</v>
+        <v>24818</v>
       </c>
       <c r="E5" s="7">
-        <v>71314</v>
+        <v>69951</v>
       </c>
       <c r="F5" s="8" t="str">
-        <v>83.06%</v>
+        <v>73.81%</v>
       </c>
       <c r="G5" s="6">
-        <v>173361</v>
+        <v>235063</v>
       </c>
       <c r="H5" s="6">
-        <v>35519</v>
+        <v>89333</v>
       </c>
       <c r="I5" s="7">
-        <v>137842</v>
+        <v>145730</v>
       </c>
       <c r="J5" s="9">
-        <v>78.42</v>
+        <v>61.32</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
@@ -1243,19 +1243,19 @@
         <v/>
       </c>
       <c r="B6" s="11" t="str">
-        <v>Customer Support</v>
+        <v>Marketing</v>
       </c>
       <c r="C6" s="12">
-        <v>37709</v>
+        <v>90536</v>
       </c>
       <c r="D6" s="12">
-        <v>8844</v>
+        <v>43976</v>
       </c>
       <c r="E6" s="13">
-        <v>28865</v>
+        <v>46560</v>
       </c>
       <c r="F6" s="14" t="str">
-        <v>76.55%</v>
+        <v>51.43%</v>
       </c>
       <c r="G6" s="11" t="str">
         <v/>
@@ -1275,19 +1275,19 @@
         <v/>
       </c>
       <c r="B7" s="17" t="str">
-        <v>Human Resources</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C7" s="18">
-        <v>49789</v>
+        <v>49758</v>
       </c>
       <c r="D7" s="18">
-        <v>12126</v>
-      </c>
-      <c r="E7" s="19">
-        <v>37663</v>
-      </c>
-      <c r="F7" s="20" t="str">
-        <v>75.65%</v>
+        <v>20539</v>
+      </c>
+      <c r="E7" s="22">
+        <v>29219</v>
+      </c>
+      <c r="F7" s="23" t="str">
+        <v>58.72%</v>
       </c>
       <c r="G7" s="17" t="str">
         <v/>
@@ -1304,34 +1304,34 @@
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="str">
-        <v>2023-05</v>
+        <v>2023-09</v>
       </c>
       <c r="B8" s="5" t="str">
-        <v>R&amp;D</v>
+        <v>Sales</v>
       </c>
       <c r="C8" s="6">
-        <v>32193</v>
+        <v>97834</v>
       </c>
       <c r="D8" s="6">
-        <v>36414</v>
-      </c>
-      <c r="E8" s="22">
-        <v>-4221</v>
-      </c>
-      <c r="F8" s="23" t="str">
-        <v>-13.11%</v>
+        <v>28398</v>
+      </c>
+      <c r="E8" s="7">
+        <v>69436</v>
+      </c>
+      <c r="F8" s="8" t="str">
+        <v>70.97%</v>
       </c>
       <c r="G8" s="6">
-        <v>100752</v>
+        <v>160539</v>
       </c>
       <c r="H8" s="6">
-        <v>109970</v>
-      </c>
-      <c r="I8" s="22">
-        <v>-9218</v>
-      </c>
-      <c r="J8" s="24">
-        <v>-9</v>
+        <v>55075</v>
+      </c>
+      <c r="I8" s="7">
+        <v>105464</v>
+      </c>
+      <c r="J8" s="9">
+        <v>58.10666666666666</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
@@ -1339,19 +1339,19 @@
         <v/>
       </c>
       <c r="B9" s="11" t="str">
-        <v>Human Resources</v>
+        <v>Customer Support</v>
       </c>
       <c r="C9" s="12">
-        <v>40611</v>
+        <v>41614</v>
       </c>
       <c r="D9" s="12">
-        <v>44182</v>
-      </c>
-      <c r="E9" s="25">
-        <v>-3571</v>
-      </c>
-      <c r="F9" s="26" t="str">
-        <v>-8.79%</v>
+        <v>12756</v>
+      </c>
+      <c r="E9" s="13">
+        <v>28858</v>
+      </c>
+      <c r="F9" s="14" t="str">
+        <v>69.35%</v>
       </c>
       <c r="G9" s="11" t="str">
         <v/>
@@ -1371,19 +1371,19 @@
         <v/>
       </c>
       <c r="B10" s="17" t="str">
-        <v>Sales</v>
+        <v>Customer Support</v>
       </c>
       <c r="C10" s="18">
-        <v>27948</v>
+        <v>21091</v>
       </c>
       <c r="D10" s="18">
-        <v>29374</v>
-      </c>
-      <c r="E10" s="27">
-        <v>-1426</v>
-      </c>
-      <c r="F10" s="28" t="str">
-        <v>-5.1%</v>
+        <v>13921</v>
+      </c>
+      <c r="E10" s="22">
+        <v>7170</v>
+      </c>
+      <c r="F10" s="23" t="str">
+        <v>34%</v>
       </c>
       <c r="G10" s="17" t="str">
         <v/>
@@ -1403,31 +1403,31 @@
         <v>2023-07</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Marketing</v>
+        <v>Customer Support</v>
       </c>
       <c r="C11" s="6">
-        <v>11214</v>
+        <v>76540</v>
       </c>
       <c r="D11" s="6">
-        <v>8016</v>
+        <v>48543</v>
       </c>
       <c r="E11" s="7">
-        <v>3198</v>
+        <v>27997</v>
       </c>
       <c r="F11" s="8" t="str">
-        <v>28.52%</v>
+        <v>36.58%</v>
       </c>
       <c r="G11" s="6">
-        <v>164248</v>
+        <v>231917</v>
       </c>
       <c r="H11" s="6">
-        <v>63972</v>
+        <v>120737</v>
       </c>
       <c r="I11" s="7">
-        <v>100276</v>
+        <v>111180</v>
       </c>
       <c r="J11" s="9">
-        <v>51.78</v>
+        <v>46.943333333333335</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
@@ -1435,19 +1435,19 @@
         <v/>
       </c>
       <c r="B12" s="11" t="str">
-        <v>R&amp;D</v>
+        <v>Marketing</v>
       </c>
       <c r="C12" s="12">
-        <v>71234</v>
+        <v>92310</v>
       </c>
       <c r="D12" s="12">
-        <v>26329</v>
+        <v>37267</v>
       </c>
       <c r="E12" s="13">
-        <v>44905</v>
+        <v>55043</v>
       </c>
       <c r="F12" s="14" t="str">
-        <v>63.04%</v>
+        <v>59.63%</v>
       </c>
       <c r="G12" s="11" t="str">
         <v/>
@@ -1467,19 +1467,19 @@
         <v/>
       </c>
       <c r="B13" s="17" t="str">
-        <v>Customer Support</v>
+        <v>Human Resources</v>
       </c>
       <c r="C13" s="18">
-        <v>81800</v>
+        <v>63067</v>
       </c>
       <c r="D13" s="18">
-        <v>29627</v>
-      </c>
-      <c r="E13" s="19">
-        <v>52173</v>
-      </c>
-      <c r="F13" s="20" t="str">
-        <v>63.78%</v>
+        <v>34927</v>
+      </c>
+      <c r="E13" s="22">
+        <v>28140</v>
+      </c>
+      <c r="F13" s="23" t="str">
+        <v>44.62%</v>
       </c>
       <c r="G13" s="17" t="str">
         <v/>
@@ -1496,34 +1496,34 @@
     </row>
     <row r="14" ht="30" customHeight="1">
       <c r="A14" s="4" t="str">
-        <v>2023-01</v>
+        <v>2023-10</v>
       </c>
       <c r="B14" s="5" t="str">
-        <v>Marketing</v>
+        <v>Human Resources</v>
       </c>
       <c r="C14" s="6">
-        <v>82328</v>
+        <v>86823</v>
       </c>
       <c r="D14" s="6">
-        <v>35772</v>
+        <v>7021</v>
       </c>
       <c r="E14" s="7">
-        <v>46556</v>
+        <v>79802</v>
       </c>
       <c r="F14" s="8" t="str">
-        <v>56.55%</v>
+        <v>91.91%</v>
       </c>
       <c r="G14" s="6">
-        <v>239958</v>
+        <v>207670</v>
       </c>
       <c r="H14" s="6">
-        <v>95963</v>
+        <v>68427</v>
       </c>
       <c r="I14" s="7">
-        <v>143995</v>
+        <v>139243</v>
       </c>
       <c r="J14" s="9">
-        <v>59.77333333333333</v>
+        <v>57.053333333333335</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
@@ -1531,19 +1531,19 @@
         <v/>
       </c>
       <c r="B15" s="11" t="str">
-        <v>R&amp;D</v>
+        <v>Customer Support</v>
       </c>
       <c r="C15" s="12">
-        <v>74243</v>
+        <v>79587</v>
       </c>
       <c r="D15" s="12">
-        <v>34171</v>
+        <v>24057</v>
       </c>
       <c r="E15" s="13">
-        <v>40072</v>
+        <v>55530</v>
       </c>
       <c r="F15" s="14" t="str">
-        <v>53.97%</v>
+        <v>69.77%</v>
       </c>
       <c r="G15" s="11" t="str">
         <v/>
@@ -1563,19 +1563,19 @@
         <v/>
       </c>
       <c r="B16" s="17" t="str">
-        <v>Sales</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C16" s="18">
-        <v>83387</v>
+        <v>41260</v>
       </c>
       <c r="D16" s="18">
-        <v>26020</v>
-      </c>
-      <c r="E16" s="19">
-        <v>57367</v>
-      </c>
-      <c r="F16" s="20" t="str">
-        <v>68.8%</v>
+        <v>37349</v>
+      </c>
+      <c r="E16" s="22">
+        <v>3911</v>
+      </c>
+      <c r="F16" s="23" t="str">
+        <v>9.48%</v>
       </c>
       <c r="G16" s="17" t="str">
         <v/>
@@ -1592,34 +1592,34 @@
     </row>
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="4" t="str">
-        <v>2023-11</v>
+        <v>2023-10</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Customer Support</v>
+        <v>Sales</v>
       </c>
       <c r="C17" s="6">
-        <v>46308</v>
+        <v>19546</v>
       </c>
       <c r="D17" s="6">
-        <v>10576</v>
-      </c>
-      <c r="E17" s="7">
-        <v>35732</v>
-      </c>
-      <c r="F17" s="8" t="str">
-        <v>77.16%</v>
+        <v>33450</v>
+      </c>
+      <c r="E17" s="24">
+        <v>-13904</v>
+      </c>
+      <c r="F17" s="25" t="str">
+        <v>-71.13%</v>
       </c>
       <c r="G17" s="6">
-        <v>195746</v>
+        <v>95635</v>
       </c>
       <c r="H17" s="6">
-        <v>82991</v>
-      </c>
-      <c r="I17" s="7">
-        <v>112755</v>
-      </c>
-      <c r="J17" s="9">
-        <v>58.23666666666666</v>
+        <v>101528</v>
+      </c>
+      <c r="I17" s="24">
+        <v>-5893</v>
+      </c>
+      <c r="J17" s="26">
+        <v>-69.38666666666666</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
@@ -1630,16 +1630,16 @@
         <v>Human Resources</v>
       </c>
       <c r="C18" s="12">
-        <v>89771</v>
+        <v>13377</v>
       </c>
       <c r="D18" s="12">
-        <v>33653</v>
-      </c>
-      <c r="E18" s="13">
-        <v>56118</v>
-      </c>
-      <c r="F18" s="14" t="str">
-        <v>62.51%</v>
+        <v>38849</v>
+      </c>
+      <c r="E18" s="27">
+        <v>-25472</v>
+      </c>
+      <c r="F18" s="28" t="str">
+        <v>-190.42%</v>
       </c>
       <c r="G18" s="11" t="str">
         <v/>
@@ -1659,19 +1659,19 @@
         <v/>
       </c>
       <c r="B19" s="17" t="str">
-        <v>Sales</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C19" s="18">
-        <v>59667</v>
+        <v>62712</v>
       </c>
       <c r="D19" s="18">
-        <v>38762</v>
-      </c>
-      <c r="E19" s="19">
-        <v>20905</v>
-      </c>
-      <c r="F19" s="20" t="str">
-        <v>35.04%</v>
+        <v>29229</v>
+      </c>
+      <c r="E19" s="22">
+        <v>33483</v>
+      </c>
+      <c r="F19" s="23" t="str">
+        <v>53.39%</v>
       </c>
       <c r="G19" s="17" t="str">
         <v/>
@@ -1688,34 +1688,34 @@
     </row>
     <row r="20" ht="30" customHeight="1">
       <c r="A20" s="4" t="str">
-        <v>2023-02</v>
+        <v>2023-01</v>
       </c>
       <c r="B20" s="5" t="str">
         <v>Human Resources</v>
       </c>
       <c r="C20" s="6">
-        <v>23450</v>
+        <v>27930</v>
       </c>
       <c r="D20" s="6">
-        <v>26226</v>
-      </c>
-      <c r="E20" s="22">
-        <v>-2776</v>
-      </c>
-      <c r="F20" s="23" t="str">
-        <v>-11.84%</v>
+        <v>47091</v>
+      </c>
+      <c r="E20" s="24">
+        <v>-19161</v>
+      </c>
+      <c r="F20" s="25" t="str">
+        <v>-68.6%</v>
       </c>
       <c r="G20" s="6">
-        <v>167804</v>
+        <v>178800</v>
       </c>
       <c r="H20" s="6">
-        <v>103683</v>
+        <v>103990</v>
       </c>
       <c r="I20" s="7">
-        <v>64121</v>
+        <v>74810</v>
       </c>
       <c r="J20" s="9">
-        <v>27.110000000000003</v>
+        <v>18.823333333333338</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
@@ -1726,16 +1726,16 @@
         <v>Marketing</v>
       </c>
       <c r="C21" s="12">
-        <v>68277</v>
+        <v>77234</v>
       </c>
       <c r="D21" s="12">
-        <v>33409</v>
+        <v>36965</v>
       </c>
       <c r="E21" s="13">
-        <v>34868</v>
+        <v>40269</v>
       </c>
       <c r="F21" s="14" t="str">
-        <v>51.07%</v>
+        <v>52.14%</v>
       </c>
       <c r="G21" s="11" t="str">
         <v/>
@@ -1755,19 +1755,19 @@
         <v/>
       </c>
       <c r="B22" s="17" t="str">
-        <v>Marketing</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C22" s="18">
-        <v>76077</v>
+        <v>73636</v>
       </c>
       <c r="D22" s="18">
-        <v>44048</v>
-      </c>
-      <c r="E22" s="19">
-        <v>32029</v>
-      </c>
-      <c r="F22" s="20" t="str">
-        <v>42.1%</v>
+        <v>19934</v>
+      </c>
+      <c r="E22" s="22">
+        <v>53702</v>
+      </c>
+      <c r="F22" s="23" t="str">
+        <v>72.93%</v>
       </c>
       <c r="G22" s="17" t="str">
         <v/>
@@ -1784,34 +1784,34 @@
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="4" t="str">
-        <v>2023-12</v>
+        <v>2023-04</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>R&amp;D</v>
+        <v>Marketing</v>
       </c>
       <c r="C23" s="6">
-        <v>92425</v>
+        <v>54182</v>
       </c>
       <c r="D23" s="6">
-        <v>16015</v>
+        <v>39120</v>
       </c>
       <c r="E23" s="7">
-        <v>76410</v>
+        <v>15062</v>
       </c>
       <c r="F23" s="8" t="str">
-        <v>82.67%</v>
+        <v>27.8%</v>
       </c>
       <c r="G23" s="6">
-        <v>203460</v>
+        <v>113286</v>
       </c>
       <c r="H23" s="6">
-        <v>47716</v>
-      </c>
-      <c r="I23" s="7">
-        <v>155744</v>
-      </c>
-      <c r="J23" s="9">
-        <v>70.33</v>
+        <v>115198</v>
+      </c>
+      <c r="I23" s="24">
+        <v>-1912</v>
+      </c>
+      <c r="J23" s="26">
+        <v>-9.139999999999999</v>
       </c>
     </row>
     <row r="24" ht="30" customHeight="1">
@@ -1819,19 +1819,19 @@
         <v/>
       </c>
       <c r="B24" s="11" t="str">
-        <v>Human Resources</v>
+        <v>Marketing</v>
       </c>
       <c r="C24" s="12">
-        <v>97130</v>
+        <v>33875</v>
       </c>
       <c r="D24" s="12">
-        <v>25364</v>
-      </c>
-      <c r="E24" s="13">
-        <v>71766</v>
-      </c>
-      <c r="F24" s="14" t="str">
-        <v>73.89%</v>
+        <v>45793</v>
+      </c>
+      <c r="E24" s="27">
+        <v>-11918</v>
+      </c>
+      <c r="F24" s="28" t="str">
+        <v>-35.18%</v>
       </c>
       <c r="G24" s="11" t="str">
         <v/>
@@ -1854,16 +1854,16 @@
         <v>Customer Support</v>
       </c>
       <c r="C25" s="18">
-        <v>13905</v>
+        <v>25229</v>
       </c>
       <c r="D25" s="18">
-        <v>6337</v>
+        <v>30285</v>
       </c>
       <c r="E25" s="19">
-        <v>7568</v>
+        <v>-5056</v>
       </c>
       <c r="F25" s="20" t="str">
-        <v>54.43%</v>
+        <v>-20.04%</v>
       </c>
       <c r="G25" s="17" t="str">
         <v/>
@@ -1880,34 +1880,34 @@
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="A26" s="4" t="str">
-        <v>2023-10</v>
+        <v>2023-01</v>
       </c>
       <c r="B26" s="5" t="str">
-        <v>Customer Support</v>
+        <v>Human Resources</v>
       </c>
       <c r="C26" s="6">
-        <v>53593</v>
+        <v>67641</v>
       </c>
       <c r="D26" s="6">
-        <v>31334</v>
+        <v>30084</v>
       </c>
       <c r="E26" s="7">
-        <v>22259</v>
+        <v>37557</v>
       </c>
       <c r="F26" s="8" t="str">
-        <v>41.53%</v>
+        <v>55.52%</v>
       </c>
       <c r="G26" s="6">
-        <v>180393</v>
+        <v>129100</v>
       </c>
       <c r="H26" s="6">
-        <v>91651</v>
+        <v>100810</v>
       </c>
       <c r="I26" s="7">
-        <v>88742</v>
-      </c>
-      <c r="J26" s="9">
-        <v>47.20333333333334</v>
+        <v>28290</v>
+      </c>
+      <c r="J26" s="26">
+        <v>-44.923333333333325</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1">
@@ -1915,19 +1915,19 @@
         <v/>
       </c>
       <c r="B27" s="11" t="str">
-        <v>Marketing</v>
+        <v>Human Resources</v>
       </c>
       <c r="C27" s="12">
-        <v>44442</v>
+        <v>13826</v>
       </c>
       <c r="D27" s="12">
-        <v>25764</v>
-      </c>
-      <c r="E27" s="13">
-        <v>18678</v>
-      </c>
-      <c r="F27" s="14" t="str">
-        <v>42.03%</v>
+        <v>47105</v>
+      </c>
+      <c r="E27" s="27">
+        <v>-33279</v>
+      </c>
+      <c r="F27" s="28" t="str">
+        <v>-240.7%</v>
       </c>
       <c r="G27" s="11" t="str">
         <v/>
@@ -1947,19 +1947,19 @@
         <v/>
       </c>
       <c r="B28" s="17" t="str">
-        <v>Marketing</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C28" s="18">
-        <v>82358</v>
+        <v>47633</v>
       </c>
       <c r="D28" s="18">
-        <v>34553</v>
-      </c>
-      <c r="E28" s="19">
-        <v>47805</v>
-      </c>
-      <c r="F28" s="20" t="str">
-        <v>58.05%</v>
+        <v>23621</v>
+      </c>
+      <c r="E28" s="22">
+        <v>24012</v>
+      </c>
+      <c r="F28" s="23" t="str">
+        <v>50.41%</v>
       </c>
       <c r="G28" s="17" t="str">
         <v/>
@@ -1976,34 +1976,34 @@
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" s="4" t="str">
-        <v>2023-02</v>
+        <v>2023-09</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>Marketing</v>
+        <v>Sales</v>
       </c>
       <c r="C29" s="6">
-        <v>98001</v>
+        <v>81438</v>
       </c>
       <c r="D29" s="6">
-        <v>11096</v>
+        <v>22154</v>
       </c>
       <c r="E29" s="7">
-        <v>86905</v>
+        <v>59284</v>
       </c>
       <c r="F29" s="8" t="str">
-        <v>88.68%</v>
+        <v>72.8%</v>
       </c>
       <c r="G29" s="6">
-        <v>255646</v>
+        <v>199820</v>
       </c>
       <c r="H29" s="6">
-        <v>54890</v>
+        <v>73862</v>
       </c>
       <c r="I29" s="7">
-        <v>200756</v>
+        <v>125958</v>
       </c>
       <c r="J29" s="9">
-        <v>77.25333333333333</v>
+        <v>56.09</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1">
@@ -2011,19 +2011,19 @@
         <v/>
       </c>
       <c r="B30" s="11" t="str">
-        <v>Marketing</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C30" s="12">
-        <v>81244</v>
+        <v>70790</v>
       </c>
       <c r="D30" s="12">
-        <v>5118</v>
+        <v>5988</v>
       </c>
       <c r="E30" s="13">
-        <v>76126</v>
+        <v>64802</v>
       </c>
       <c r="F30" s="14" t="str">
-        <v>93.7%</v>
+        <v>91.54%</v>
       </c>
       <c r="G30" s="11" t="str">
         <v/>
@@ -2043,19 +2043,19 @@
         <v/>
       </c>
       <c r="B31" s="17" t="str">
-        <v>Customer Support</v>
+        <v>Human Resources</v>
       </c>
       <c r="C31" s="18">
-        <v>76401</v>
+        <v>47592</v>
       </c>
       <c r="D31" s="18">
-        <v>38676</v>
-      </c>
-      <c r="E31" s="19">
-        <v>37725</v>
-      </c>
-      <c r="F31" s="20" t="str">
-        <v>49.38%</v>
+        <v>45720</v>
+      </c>
+      <c r="E31" s="22">
+        <v>1872</v>
+      </c>
+      <c r="F31" s="23" t="str">
+        <v>3.93%</v>
       </c>
       <c r="G31" s="17" t="str">
         <v/>
@@ -2072,16 +2072,16 @@
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="G32" s="29">
-        <v>1853501</v>
+        <v>1770373</v>
       </c>
       <c r="H32" s="29">
-        <v>741125</v>
+        <v>949372</v>
       </c>
       <c r="I32" s="30">
-        <v>1112376</v>
+        <v>821001</v>
       </c>
       <c r="J32" s="31">
-        <v>53.03366666666666</v>
+        <v>20.867333333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implement cell format shared presets
</commit_message>
<xml_diff>
--- a/examples/financial-report.xlsx
+++ b/examples/financial-report.xlsx
@@ -78,12 +78,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <color rgb="007500"/>
+      <color rgb="FF0000"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <color rgb="007500"/>
+      <color rgb="FF0000"/>
     </font>
     <font>
       <sz val="11"/>
@@ -108,12 +108,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <color rgb="FF0000"/>
+      <color rgb="007500"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <color rgb="FF0000"/>
+      <color rgb="007500"/>
     </font>
     <font>
       <sz val="11"/>
@@ -494,6 +494,36 @@
       <top style="thin">
         <color rgb="000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000"/>
+      </top>
       <bottom style="medium">
         <color rgb="000000"/>
       </bottom>
@@ -552,36 +582,6 @@
         <color rgb="000000"/>
       </right>
       <top style="medium">
-        <color rgb="000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="000000"/>
-      </right>
-      <top style="thin">
         <color rgb="000000"/>
       </top>
       <bottom style="thin">
@@ -711,13 +711,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="175" fontId="17" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyNumberFormat="1" applyAlignment="1">
@@ -1112,34 +1112,34 @@
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="4" t="str">
-        <v>2023-05</v>
+        <v>2023-04</v>
       </c>
       <c r="B2" s="5" t="str">
         <v>Marketing</v>
       </c>
       <c r="C2" s="6">
-        <v>84367</v>
+        <v>99559</v>
       </c>
       <c r="D2" s="6">
-        <v>38132</v>
+        <v>33606</v>
       </c>
       <c r="E2" s="7">
-        <v>46235</v>
+        <v>65953</v>
       </c>
       <c r="F2" s="8" t="str">
-        <v>54.8%</v>
+        <v>66.25%</v>
       </c>
       <c r="G2" s="6">
-        <v>218543</v>
+        <v>178808</v>
       </c>
       <c r="H2" s="6">
-        <v>120412</v>
+        <v>121919</v>
       </c>
       <c r="I2" s="7">
-        <v>98131</v>
+        <v>56889</v>
       </c>
       <c r="J2" s="9">
-        <v>33.78666666666667</v>
+        <v>13.836666666666666</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
@@ -1147,19 +1147,19 @@
         <v/>
       </c>
       <c r="B3" s="11" t="str">
-        <v>Marketing</v>
+        <v>Human Resources</v>
       </c>
       <c r="C3" s="12">
-        <v>93734</v>
+        <v>36240</v>
       </c>
       <c r="D3" s="12">
-        <v>35578</v>
+        <v>44692</v>
       </c>
       <c r="E3" s="13">
-        <v>58156</v>
+        <v>-8452</v>
       </c>
       <c r="F3" s="14" t="str">
-        <v>62.04%</v>
+        <v>-23.32%</v>
       </c>
       <c r="G3" s="11" t="str">
         <v/>
@@ -1179,19 +1179,19 @@
         <v/>
       </c>
       <c r="B4" s="17" t="str">
-        <v>Marketing</v>
+        <v>Human Resources</v>
       </c>
       <c r="C4" s="18">
-        <v>40442</v>
+        <v>43009</v>
       </c>
       <c r="D4" s="18">
-        <v>46702</v>
+        <v>43621</v>
       </c>
       <c r="E4" s="19">
-        <v>-6260</v>
+        <v>-612</v>
       </c>
       <c r="F4" s="20" t="str">
-        <v>-15.48%</v>
+        <v>-1.42%</v>
       </c>
       <c r="G4" s="17" t="str">
         <v/>
@@ -1208,34 +1208,34 @@
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="4" t="str">
-        <v>2023-07</v>
+        <v>2023-09</v>
       </c>
       <c r="B5" s="5" t="str">
         <v>R&amp;D</v>
       </c>
       <c r="C5" s="6">
-        <v>94769</v>
+        <v>47392</v>
       </c>
       <c r="D5" s="6">
-        <v>24818</v>
+        <v>37876</v>
       </c>
       <c r="E5" s="7">
-        <v>69951</v>
+        <v>9516</v>
       </c>
       <c r="F5" s="8" t="str">
-        <v>73.81%</v>
+        <v>20.08%</v>
       </c>
       <c r="G5" s="6">
-        <v>235063</v>
+        <v>174700</v>
       </c>
       <c r="H5" s="6">
-        <v>89333</v>
+        <v>116015</v>
       </c>
       <c r="I5" s="7">
-        <v>145730</v>
+        <v>58685</v>
       </c>
       <c r="J5" s="9">
-        <v>61.32</v>
+        <v>17.386666666666667</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
@@ -1243,19 +1243,19 @@
         <v/>
       </c>
       <c r="B6" s="11" t="str">
-        <v>Marketing</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C6" s="12">
-        <v>90536</v>
+        <v>92570</v>
       </c>
       <c r="D6" s="12">
-        <v>43976</v>
-      </c>
-      <c r="E6" s="13">
-        <v>46560</v>
-      </c>
-      <c r="F6" s="14" t="str">
-        <v>51.43%</v>
+        <v>31700</v>
+      </c>
+      <c r="E6" s="22">
+        <v>60870</v>
+      </c>
+      <c r="F6" s="23" t="str">
+        <v>65.76%</v>
       </c>
       <c r="G6" s="11" t="str">
         <v/>
@@ -1278,16 +1278,16 @@
         <v>R&amp;D</v>
       </c>
       <c r="C7" s="18">
-        <v>49758</v>
+        <v>34738</v>
       </c>
       <c r="D7" s="18">
-        <v>20539</v>
-      </c>
-      <c r="E7" s="22">
-        <v>29219</v>
-      </c>
-      <c r="F7" s="23" t="str">
-        <v>58.72%</v>
+        <v>46439</v>
+      </c>
+      <c r="E7" s="19">
+        <v>-11701</v>
+      </c>
+      <c r="F7" s="20" t="str">
+        <v>-33.68%</v>
       </c>
       <c r="G7" s="17" t="str">
         <v/>
@@ -1304,34 +1304,34 @@
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="str">
-        <v>2023-09</v>
+        <v>2023-10</v>
       </c>
       <c r="B8" s="5" t="str">
-        <v>Sales</v>
+        <v>Customer Support</v>
       </c>
       <c r="C8" s="6">
-        <v>97834</v>
+        <v>66005</v>
       </c>
       <c r="D8" s="6">
-        <v>28398</v>
+        <v>40581</v>
       </c>
       <c r="E8" s="7">
-        <v>69436</v>
+        <v>25424</v>
       </c>
       <c r="F8" s="8" t="str">
-        <v>70.97%</v>
+        <v>38.52%</v>
       </c>
       <c r="G8" s="6">
-        <v>160539</v>
+        <v>197035</v>
       </c>
       <c r="H8" s="6">
-        <v>55075</v>
+        <v>134587</v>
       </c>
       <c r="I8" s="7">
-        <v>105464</v>
+        <v>62448</v>
       </c>
       <c r="J8" s="9">
-        <v>58.10666666666666</v>
+        <v>30.736666666666668</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
@@ -1339,19 +1339,19 @@
         <v/>
       </c>
       <c r="B9" s="11" t="str">
-        <v>Customer Support</v>
+        <v>Sales</v>
       </c>
       <c r="C9" s="12">
-        <v>41614</v>
+        <v>74440</v>
       </c>
       <c r="D9" s="12">
-        <v>12756</v>
-      </c>
-      <c r="E9" s="13">
-        <v>28858</v>
-      </c>
-      <c r="F9" s="14" t="str">
-        <v>69.35%</v>
+        <v>46729</v>
+      </c>
+      <c r="E9" s="22">
+        <v>27711</v>
+      </c>
+      <c r="F9" s="23" t="str">
+        <v>37.23%</v>
       </c>
       <c r="G9" s="11" t="str">
         <v/>
@@ -1374,16 +1374,16 @@
         <v>Customer Support</v>
       </c>
       <c r="C10" s="18">
-        <v>21091</v>
+        <v>56590</v>
       </c>
       <c r="D10" s="18">
-        <v>13921</v>
-      </c>
-      <c r="E10" s="22">
-        <v>7170</v>
-      </c>
-      <c r="F10" s="23" t="str">
-        <v>34%</v>
+        <v>47277</v>
+      </c>
+      <c r="E10" s="24">
+        <v>9313</v>
+      </c>
+      <c r="F10" s="25" t="str">
+        <v>16.46%</v>
       </c>
       <c r="G10" s="17" t="str">
         <v/>
@@ -1400,34 +1400,34 @@
     </row>
     <row r="11" ht="30" customHeight="1">
       <c r="A11" s="4" t="str">
-        <v>2023-07</v>
+        <v>2023-03</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Customer Support</v>
+        <v>Sales</v>
       </c>
       <c r="C11" s="6">
-        <v>76540</v>
+        <v>65766</v>
       </c>
       <c r="D11" s="6">
-        <v>48543</v>
+        <v>6351</v>
       </c>
       <c r="E11" s="7">
-        <v>27997</v>
+        <v>59415</v>
       </c>
       <c r="F11" s="8" t="str">
-        <v>36.58%</v>
+        <v>90.34%</v>
       </c>
       <c r="G11" s="6">
-        <v>231917</v>
+        <v>154391</v>
       </c>
       <c r="H11" s="6">
-        <v>120737</v>
+        <v>100408</v>
       </c>
       <c r="I11" s="7">
-        <v>111180</v>
+        <v>53983</v>
       </c>
       <c r="J11" s="9">
-        <v>46.943333333333335</v>
+        <v>26.040000000000003</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
@@ -1435,19 +1435,19 @@
         <v/>
       </c>
       <c r="B12" s="11" t="str">
-        <v>Marketing</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C12" s="12">
-        <v>92310</v>
+        <v>43950</v>
       </c>
       <c r="D12" s="12">
-        <v>37267</v>
+        <v>45585</v>
       </c>
       <c r="E12" s="13">
-        <v>55043</v>
+        <v>-1635</v>
       </c>
       <c r="F12" s="14" t="str">
-        <v>59.63%</v>
+        <v>-3.72%</v>
       </c>
       <c r="G12" s="11" t="str">
         <v/>
@@ -1467,19 +1467,19 @@
         <v/>
       </c>
       <c r="B13" s="17" t="str">
-        <v>Human Resources</v>
+        <v>Customer Support</v>
       </c>
       <c r="C13" s="18">
-        <v>63067</v>
+        <v>44675</v>
       </c>
       <c r="D13" s="18">
-        <v>34927</v>
-      </c>
-      <c r="E13" s="22">
-        <v>28140</v>
-      </c>
-      <c r="F13" s="23" t="str">
-        <v>44.62%</v>
+        <v>48472</v>
+      </c>
+      <c r="E13" s="19">
+        <v>-3797</v>
+      </c>
+      <c r="F13" s="20" t="str">
+        <v>-8.5%</v>
       </c>
       <c r="G13" s="17" t="str">
         <v/>
@@ -1499,31 +1499,31 @@
         <v>2023-10</v>
       </c>
       <c r="B14" s="5" t="str">
-        <v>Human Resources</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C14" s="6">
-        <v>86823</v>
+        <v>25523</v>
       </c>
       <c r="D14" s="6">
-        <v>7021</v>
-      </c>
-      <c r="E14" s="7">
-        <v>79802</v>
-      </c>
-      <c r="F14" s="8" t="str">
-        <v>91.91%</v>
+        <v>45948</v>
+      </c>
+      <c r="E14" s="26">
+        <v>-20425</v>
+      </c>
+      <c r="F14" s="27" t="str">
+        <v>-80.03%</v>
       </c>
       <c r="G14" s="6">
-        <v>207670</v>
+        <v>95012</v>
       </c>
       <c r="H14" s="6">
-        <v>68427</v>
-      </c>
-      <c r="I14" s="7">
-        <v>139243</v>
-      </c>
-      <c r="J14" s="9">
-        <v>57.053333333333335</v>
+        <v>133005</v>
+      </c>
+      <c r="I14" s="26">
+        <v>-37993</v>
+      </c>
+      <c r="J14" s="28">
+        <v>-51.35666666666666</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
@@ -1531,19 +1531,19 @@
         <v/>
       </c>
       <c r="B15" s="11" t="str">
-        <v>Customer Support</v>
+        <v>Human Resources</v>
       </c>
       <c r="C15" s="12">
-        <v>79587</v>
+        <v>43596</v>
       </c>
       <c r="D15" s="12">
-        <v>24057</v>
-      </c>
-      <c r="E15" s="13">
-        <v>55530</v>
-      </c>
-      <c r="F15" s="14" t="str">
-        <v>69.77%</v>
+        <v>39648</v>
+      </c>
+      <c r="E15" s="22">
+        <v>3948</v>
+      </c>
+      <c r="F15" s="23" t="str">
+        <v>9.06%</v>
       </c>
       <c r="G15" s="11" t="str">
         <v/>
@@ -1563,19 +1563,19 @@
         <v/>
       </c>
       <c r="B16" s="17" t="str">
-        <v>R&amp;D</v>
+        <v>Marketing</v>
       </c>
       <c r="C16" s="18">
-        <v>41260</v>
+        <v>25893</v>
       </c>
       <c r="D16" s="18">
-        <v>37349</v>
-      </c>
-      <c r="E16" s="22">
-        <v>3911</v>
-      </c>
-      <c r="F16" s="23" t="str">
-        <v>9.48%</v>
+        <v>47409</v>
+      </c>
+      <c r="E16" s="19">
+        <v>-21516</v>
+      </c>
+      <c r="F16" s="20" t="str">
+        <v>-83.1%</v>
       </c>
       <c r="G16" s="17" t="str">
         <v/>
@@ -1592,34 +1592,34 @@
     </row>
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="4" t="str">
-        <v>2023-10</v>
+        <v>2023-05</v>
       </c>
       <c r="B17" s="5" t="str">
         <v>Sales</v>
       </c>
       <c r="C17" s="6">
-        <v>19546</v>
+        <v>12624</v>
       </c>
       <c r="D17" s="6">
-        <v>33450</v>
-      </c>
-      <c r="E17" s="24">
-        <v>-13904</v>
-      </c>
-      <c r="F17" s="25" t="str">
-        <v>-71.13%</v>
+        <v>19448</v>
+      </c>
+      <c r="E17" s="26">
+        <v>-6824</v>
+      </c>
+      <c r="F17" s="27" t="str">
+        <v>-54.06%</v>
       </c>
       <c r="G17" s="6">
-        <v>95635</v>
+        <v>140847</v>
       </c>
       <c r="H17" s="6">
-        <v>101528</v>
-      </c>
-      <c r="I17" s="24">
-        <v>-5893</v>
-      </c>
-      <c r="J17" s="26">
-        <v>-69.38666666666666</v>
+        <v>71511</v>
+      </c>
+      <c r="I17" s="7">
+        <v>69336</v>
+      </c>
+      <c r="J17" s="9">
+        <v>14.466666666666663</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
@@ -1627,19 +1627,19 @@
         <v/>
       </c>
       <c r="B18" s="11" t="str">
-        <v>Human Resources</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C18" s="12">
-        <v>13377</v>
+        <v>45738</v>
       </c>
       <c r="D18" s="12">
-        <v>38849</v>
-      </c>
-      <c r="E18" s="27">
-        <v>-25472</v>
-      </c>
-      <c r="F18" s="28" t="str">
-        <v>-190.42%</v>
+        <v>40478</v>
+      </c>
+      <c r="E18" s="22">
+        <v>5260</v>
+      </c>
+      <c r="F18" s="23" t="str">
+        <v>11.5%</v>
       </c>
       <c r="G18" s="11" t="str">
         <v/>
@@ -1659,19 +1659,19 @@
         <v/>
       </c>
       <c r="B19" s="17" t="str">
-        <v>R&amp;D</v>
+        <v>Customer Support</v>
       </c>
       <c r="C19" s="18">
-        <v>62712</v>
+        <v>82485</v>
       </c>
       <c r="D19" s="18">
-        <v>29229</v>
-      </c>
-      <c r="E19" s="22">
-        <v>33483</v>
-      </c>
-      <c r="F19" s="23" t="str">
-        <v>53.39%</v>
+        <v>11585</v>
+      </c>
+      <c r="E19" s="24">
+        <v>70900</v>
+      </c>
+      <c r="F19" s="25" t="str">
+        <v>85.96%</v>
       </c>
       <c r="G19" s="17" t="str">
         <v/>
@@ -1688,34 +1688,34 @@
     </row>
     <row r="20" ht="30" customHeight="1">
       <c r="A20" s="4" t="str">
-        <v>2023-01</v>
+        <v>2023-11</v>
       </c>
       <c r="B20" s="5" t="str">
-        <v>Human Resources</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C20" s="6">
-        <v>27930</v>
+        <v>67194</v>
       </c>
       <c r="D20" s="6">
-        <v>47091</v>
-      </c>
-      <c r="E20" s="24">
-        <v>-19161</v>
-      </c>
-      <c r="F20" s="25" t="str">
-        <v>-68.6%</v>
+        <v>47962</v>
+      </c>
+      <c r="E20" s="7">
+        <v>19232</v>
+      </c>
+      <c r="F20" s="8" t="str">
+        <v>28.62%</v>
       </c>
       <c r="G20" s="6">
-        <v>178800</v>
+        <v>144934</v>
       </c>
       <c r="H20" s="6">
-        <v>103990</v>
+        <v>127651</v>
       </c>
       <c r="I20" s="7">
-        <v>74810</v>
-      </c>
-      <c r="J20" s="9">
-        <v>18.823333333333338</v>
+        <v>17283</v>
+      </c>
+      <c r="J20" s="28">
+        <v>-38.39</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
@@ -1723,19 +1723,19 @@
         <v/>
       </c>
       <c r="B21" s="11" t="str">
-        <v>Marketing</v>
+        <v>Sales</v>
       </c>
       <c r="C21" s="12">
-        <v>77234</v>
+        <v>61108</v>
       </c>
       <c r="D21" s="12">
-        <v>36965</v>
-      </c>
-      <c r="E21" s="13">
-        <v>40269</v>
-      </c>
-      <c r="F21" s="14" t="str">
-        <v>52.14%</v>
+        <v>30927</v>
+      </c>
+      <c r="E21" s="22">
+        <v>30181</v>
+      </c>
+      <c r="F21" s="23" t="str">
+        <v>49.39%</v>
       </c>
       <c r="G21" s="11" t="str">
         <v/>
@@ -1755,19 +1755,19 @@
         <v/>
       </c>
       <c r="B22" s="17" t="str">
-        <v>R&amp;D</v>
+        <v>Sales</v>
       </c>
       <c r="C22" s="18">
-        <v>73636</v>
+        <v>16632</v>
       </c>
       <c r="D22" s="18">
-        <v>19934</v>
-      </c>
-      <c r="E22" s="22">
-        <v>53702</v>
-      </c>
-      <c r="F22" s="23" t="str">
-        <v>72.93%</v>
+        <v>48762</v>
+      </c>
+      <c r="E22" s="19">
+        <v>-32130</v>
+      </c>
+      <c r="F22" s="20" t="str">
+        <v>-193.18%</v>
       </c>
       <c r="G22" s="17" t="str">
         <v/>
@@ -1784,34 +1784,34 @@
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="4" t="str">
-        <v>2023-04</v>
+        <v>2023-10</v>
       </c>
       <c r="B23" s="5" t="str">
         <v>Marketing</v>
       </c>
       <c r="C23" s="6">
-        <v>54182</v>
+        <v>81697</v>
       </c>
       <c r="D23" s="6">
-        <v>39120</v>
+        <v>28754</v>
       </c>
       <c r="E23" s="7">
-        <v>15062</v>
+        <v>52943</v>
       </c>
       <c r="F23" s="8" t="str">
-        <v>27.8%</v>
+        <v>64.8%</v>
       </c>
       <c r="G23" s="6">
-        <v>113286</v>
+        <v>209145</v>
       </c>
       <c r="H23" s="6">
-        <v>115198</v>
-      </c>
-      <c r="I23" s="24">
-        <v>-1912</v>
-      </c>
-      <c r="J23" s="26">
-        <v>-9.139999999999999</v>
+        <v>104697</v>
+      </c>
+      <c r="I23" s="7">
+        <v>104448</v>
+      </c>
+      <c r="J23" s="9">
+        <v>36.21333333333333</v>
       </c>
     </row>
     <row r="24" ht="30" customHeight="1">
@@ -1819,19 +1819,19 @@
         <v/>
       </c>
       <c r="B24" s="11" t="str">
-        <v>Marketing</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C24" s="12">
-        <v>33875</v>
+        <v>98040</v>
       </c>
       <c r="D24" s="12">
-        <v>45793</v>
-      </c>
-      <c r="E24" s="27">
-        <v>-11918</v>
-      </c>
-      <c r="F24" s="28" t="str">
-        <v>-35.18%</v>
+        <v>42882</v>
+      </c>
+      <c r="E24" s="22">
+        <v>55158</v>
+      </c>
+      <c r="F24" s="23" t="str">
+        <v>56.26%</v>
       </c>
       <c r="G24" s="11" t="str">
         <v/>
@@ -1851,19 +1851,19 @@
         <v/>
       </c>
       <c r="B25" s="17" t="str">
-        <v>Customer Support</v>
+        <v>Sales</v>
       </c>
       <c r="C25" s="18">
-        <v>25229</v>
+        <v>29408</v>
       </c>
       <c r="D25" s="18">
-        <v>30285</v>
+        <v>33061</v>
       </c>
       <c r="E25" s="19">
-        <v>-5056</v>
+        <v>-3653</v>
       </c>
       <c r="F25" s="20" t="str">
-        <v>-20.04%</v>
+        <v>-12.42%</v>
       </c>
       <c r="G25" s="17" t="str">
         <v/>
@@ -1880,34 +1880,34 @@
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="A26" s="4" t="str">
-        <v>2023-01</v>
+        <v>2023-09</v>
       </c>
       <c r="B26" s="5" t="str">
-        <v>Human Resources</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C26" s="6">
-        <v>67641</v>
+        <v>53606</v>
       </c>
       <c r="D26" s="6">
-        <v>30084</v>
+        <v>6800</v>
       </c>
       <c r="E26" s="7">
-        <v>37557</v>
+        <v>46806</v>
       </c>
       <c r="F26" s="8" t="str">
-        <v>55.52%</v>
+        <v>87.31%</v>
       </c>
       <c r="G26" s="6">
-        <v>129100</v>
+        <v>159235</v>
       </c>
       <c r="H26" s="6">
-        <v>100810</v>
+        <v>66799</v>
       </c>
       <c r="I26" s="7">
-        <v>28290</v>
-      </c>
-      <c r="J26" s="26">
-        <v>-44.923333333333325</v>
+        <v>92436</v>
+      </c>
+      <c r="J26" s="9">
+        <v>58.553333333333335</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1">
@@ -1915,19 +1915,19 @@
         <v/>
       </c>
       <c r="B27" s="11" t="str">
-        <v>Human Resources</v>
+        <v>Marketing</v>
       </c>
       <c r="C27" s="12">
-        <v>13826</v>
+        <v>56996</v>
       </c>
       <c r="D27" s="12">
-        <v>47105</v>
-      </c>
-      <c r="E27" s="27">
-        <v>-33279</v>
-      </c>
-      <c r="F27" s="28" t="str">
-        <v>-240.7%</v>
+        <v>38845</v>
+      </c>
+      <c r="E27" s="22">
+        <v>18151</v>
+      </c>
+      <c r="F27" s="23" t="str">
+        <v>31.85%</v>
       </c>
       <c r="G27" s="11" t="str">
         <v/>
@@ -1947,19 +1947,19 @@
         <v/>
       </c>
       <c r="B28" s="17" t="str">
-        <v>R&amp;D</v>
+        <v>Customer Support</v>
       </c>
       <c r="C28" s="18">
-        <v>47633</v>
+        <v>48633</v>
       </c>
       <c r="D28" s="18">
-        <v>23621</v>
-      </c>
-      <c r="E28" s="22">
-        <v>24012</v>
-      </c>
-      <c r="F28" s="23" t="str">
-        <v>50.41%</v>
+        <v>21154</v>
+      </c>
+      <c r="E28" s="24">
+        <v>27479</v>
+      </c>
+      <c r="F28" s="25" t="str">
+        <v>56.5%</v>
       </c>
       <c r="G28" s="17" t="str">
         <v/>
@@ -1976,34 +1976,34 @@
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" s="4" t="str">
-        <v>2023-09</v>
+        <v>2023-11</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>Sales</v>
+        <v>Customer Support</v>
       </c>
       <c r="C29" s="6">
-        <v>81438</v>
+        <v>48056</v>
       </c>
       <c r="D29" s="6">
-        <v>22154</v>
+        <v>30383</v>
       </c>
       <c r="E29" s="7">
-        <v>59284</v>
+        <v>17673</v>
       </c>
       <c r="F29" s="8" t="str">
-        <v>72.8%</v>
+        <v>36.78%</v>
       </c>
       <c r="G29" s="6">
-        <v>199820</v>
+        <v>138701</v>
       </c>
       <c r="H29" s="6">
-        <v>73862</v>
+        <v>69900</v>
       </c>
       <c r="I29" s="7">
-        <v>125958</v>
+        <v>68801</v>
       </c>
       <c r="J29" s="9">
-        <v>56.09</v>
+        <v>45.126666666666665</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1">
@@ -2011,19 +2011,19 @@
         <v/>
       </c>
       <c r="B30" s="11" t="str">
-        <v>R&amp;D</v>
+        <v>Marketing</v>
       </c>
       <c r="C30" s="12">
-        <v>70790</v>
+        <v>57529</v>
       </c>
       <c r="D30" s="12">
-        <v>5988</v>
-      </c>
-      <c r="E30" s="13">
-        <v>64802</v>
-      </c>
-      <c r="F30" s="14" t="str">
-        <v>91.54%</v>
+        <v>13987</v>
+      </c>
+      <c r="E30" s="22">
+        <v>43542</v>
+      </c>
+      <c r="F30" s="23" t="str">
+        <v>75.69%</v>
       </c>
       <c r="G30" s="11" t="str">
         <v/>
@@ -2046,16 +2046,16 @@
         <v>Human Resources</v>
       </c>
       <c r="C31" s="18">
-        <v>47592</v>
+        <v>33116</v>
       </c>
       <c r="D31" s="18">
-        <v>45720</v>
-      </c>
-      <c r="E31" s="22">
-        <v>1872</v>
-      </c>
-      <c r="F31" s="23" t="str">
-        <v>3.93%</v>
+        <v>25530</v>
+      </c>
+      <c r="E31" s="24">
+        <v>7586</v>
+      </c>
+      <c r="F31" s="25" t="str">
+        <v>22.91%</v>
       </c>
       <c r="G31" s="17" t="str">
         <v/>
@@ -2072,16 +2072,16 @@
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="G32" s="29">
-        <v>1770373</v>
+        <v>1592808</v>
       </c>
       <c r="H32" s="29">
-        <v>949372</v>
+        <v>1046492</v>
       </c>
       <c r="I32" s="30">
-        <v>821001</v>
+        <v>546316</v>
       </c>
       <c r="J32" s="31">
-        <v>20.867333333333335</v>
+        <v>15.261333333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implement parametric schema-level formatters
</commit_message>
<xml_diff>
--- a/examples/financial-report.xlsx
+++ b/examples/financial-report.xlsx
@@ -78,7 +78,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <color rgb="FF0000"/>
+      <color rgb="007500"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <color rgb="007500"/>
     </font>
     <font>
       <sz val="11"/>
@@ -98,12 +103,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <color rgb="007500"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <color rgb="007500"/>
+      <color rgb="FF0000"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1112,34 +1112,34 @@
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="4" t="str">
-        <v>2023-04</v>
+        <v>2023-05</v>
       </c>
       <c r="B2" s="5" t="str">
-        <v>Marketing</v>
+        <v>Human Resources</v>
       </c>
       <c r="C2" s="6">
-        <v>99559</v>
+        <v>80336</v>
       </c>
       <c r="D2" s="6">
-        <v>33606</v>
+        <v>21916</v>
       </c>
       <c r="E2" s="7">
-        <v>65953</v>
+        <v>58420</v>
       </c>
       <c r="F2" s="8" t="str">
-        <v>66.25%</v>
+        <v>72.72%</v>
       </c>
       <c r="G2" s="6">
-        <v>178808</v>
+        <v>194223</v>
       </c>
       <c r="H2" s="6">
-        <v>121919</v>
+        <v>56200</v>
       </c>
       <c r="I2" s="7">
-        <v>56889</v>
+        <v>138023</v>
       </c>
       <c r="J2" s="9">
-        <v>13.836666666666666</v>
+        <v>32.72666666666667</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
@@ -1147,19 +1147,19 @@
         <v/>
       </c>
       <c r="B3" s="11" t="str">
-        <v>Human Resources</v>
+        <v>Sales</v>
       </c>
       <c r="C3" s="12">
-        <v>36240</v>
+        <v>97976</v>
       </c>
       <c r="D3" s="12">
-        <v>44692</v>
+        <v>7774</v>
       </c>
       <c r="E3" s="13">
-        <v>-8452</v>
+        <v>90202</v>
       </c>
       <c r="F3" s="14" t="str">
-        <v>-23.32%</v>
+        <v>92.07%</v>
       </c>
       <c r="G3" s="11" t="str">
         <v/>
@@ -1179,19 +1179,19 @@
         <v/>
       </c>
       <c r="B4" s="17" t="str">
-        <v>Human Resources</v>
+        <v>Customer Support</v>
       </c>
       <c r="C4" s="18">
-        <v>43009</v>
+        <v>15911</v>
       </c>
       <c r="D4" s="18">
-        <v>43621</v>
+        <v>26510</v>
       </c>
       <c r="E4" s="19">
-        <v>-612</v>
+        <v>-10599</v>
       </c>
       <c r="F4" s="20" t="str">
-        <v>-1.42%</v>
+        <v>-66.61%</v>
       </c>
       <c r="G4" s="17" t="str">
         <v/>
@@ -1208,34 +1208,34 @@
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="4" t="str">
-        <v>2023-09</v>
+        <v>2023-05</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>R&amp;D</v>
+        <v>Sales</v>
       </c>
       <c r="C5" s="6">
-        <v>47392</v>
+        <v>64442</v>
       </c>
       <c r="D5" s="6">
-        <v>37876</v>
+        <v>38483</v>
       </c>
       <c r="E5" s="7">
-        <v>9516</v>
+        <v>25959</v>
       </c>
       <c r="F5" s="8" t="str">
-        <v>20.08%</v>
+        <v>40.28%</v>
       </c>
       <c r="G5" s="6">
-        <v>174700</v>
+        <v>145047</v>
       </c>
       <c r="H5" s="6">
-        <v>116015</v>
+        <v>118052</v>
       </c>
       <c r="I5" s="7">
-        <v>58685</v>
+        <v>26995</v>
       </c>
       <c r="J5" s="9">
-        <v>17.386666666666667</v>
+        <v>14.256666666666668</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
@@ -1246,16 +1246,16 @@
         <v>R&amp;D</v>
       </c>
       <c r="C6" s="12">
-        <v>92570</v>
+        <v>39864</v>
       </c>
       <c r="D6" s="12">
-        <v>31700</v>
+        <v>40866</v>
       </c>
       <c r="E6" s="22">
-        <v>60870</v>
+        <v>-1002</v>
       </c>
       <c r="F6" s="23" t="str">
-        <v>65.76%</v>
+        <v>-2.51%</v>
       </c>
       <c r="G6" s="11" t="str">
         <v/>
@@ -1278,16 +1278,16 @@
         <v>R&amp;D</v>
       </c>
       <c r="C7" s="18">
-        <v>34738</v>
+        <v>40741</v>
       </c>
       <c r="D7" s="18">
-        <v>46439</v>
-      </c>
-      <c r="E7" s="19">
-        <v>-11701</v>
-      </c>
-      <c r="F7" s="20" t="str">
-        <v>-33.68%</v>
+        <v>38703</v>
+      </c>
+      <c r="E7" s="24">
+        <v>2038</v>
+      </c>
+      <c r="F7" s="25" t="str">
+        <v>5%</v>
       </c>
       <c r="G7" s="17" t="str">
         <v/>
@@ -1304,34 +1304,34 @@
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="str">
-        <v>2023-10</v>
+        <v>2023-12</v>
       </c>
       <c r="B8" s="5" t="str">
-        <v>Customer Support</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C8" s="6">
-        <v>66005</v>
+        <v>76606</v>
       </c>
       <c r="D8" s="6">
-        <v>40581</v>
+        <v>47128</v>
       </c>
       <c r="E8" s="7">
-        <v>25424</v>
+        <v>29478</v>
       </c>
       <c r="F8" s="8" t="str">
-        <v>38.52%</v>
+        <v>38.48%</v>
       </c>
       <c r="G8" s="6">
-        <v>197035</v>
+        <v>195532</v>
       </c>
       <c r="H8" s="6">
-        <v>134587</v>
+        <v>101061</v>
       </c>
       <c r="I8" s="7">
-        <v>62448</v>
+        <v>94471</v>
       </c>
       <c r="J8" s="9">
-        <v>30.736666666666668</v>
+        <v>49.423333333333325</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
@@ -1339,19 +1339,19 @@
         <v/>
       </c>
       <c r="B9" s="11" t="str">
-        <v>Sales</v>
+        <v>Customer Support</v>
       </c>
       <c r="C9" s="12">
-        <v>74440</v>
+        <v>62937</v>
       </c>
       <c r="D9" s="12">
-        <v>46729</v>
-      </c>
-      <c r="E9" s="22">
-        <v>27711</v>
-      </c>
-      <c r="F9" s="23" t="str">
-        <v>37.23%</v>
+        <v>31017</v>
+      </c>
+      <c r="E9" s="13">
+        <v>31920</v>
+      </c>
+      <c r="F9" s="14" t="str">
+        <v>50.72%</v>
       </c>
       <c r="G9" s="11" t="str">
         <v/>
@@ -1371,19 +1371,19 @@
         <v/>
       </c>
       <c r="B10" s="17" t="str">
-        <v>Customer Support</v>
+        <v>Sales</v>
       </c>
       <c r="C10" s="18">
-        <v>56590</v>
+        <v>55989</v>
       </c>
       <c r="D10" s="18">
-        <v>47277</v>
+        <v>22916</v>
       </c>
       <c r="E10" s="24">
-        <v>9313</v>
+        <v>33073</v>
       </c>
       <c r="F10" s="25" t="str">
-        <v>16.46%</v>
+        <v>59.07%</v>
       </c>
       <c r="G10" s="17" t="str">
         <v/>
@@ -1400,34 +1400,34 @@
     </row>
     <row r="11" ht="30" customHeight="1">
       <c r="A11" s="4" t="str">
-        <v>2023-03</v>
+        <v>2023-09</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Sales</v>
+        <v>Customer Support</v>
       </c>
       <c r="C11" s="6">
-        <v>65766</v>
+        <v>59106</v>
       </c>
       <c r="D11" s="6">
-        <v>6351</v>
+        <v>41396</v>
       </c>
       <c r="E11" s="7">
-        <v>59415</v>
+        <v>17710</v>
       </c>
       <c r="F11" s="8" t="str">
-        <v>90.34%</v>
+        <v>29.96%</v>
       </c>
       <c r="G11" s="6">
-        <v>154391</v>
+        <v>168847</v>
       </c>
       <c r="H11" s="6">
-        <v>100408</v>
+        <v>63633</v>
       </c>
       <c r="I11" s="7">
-        <v>53983</v>
+        <v>105214</v>
       </c>
       <c r="J11" s="9">
-        <v>26.040000000000003</v>
+        <v>62.330000000000005</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
@@ -1438,16 +1438,16 @@
         <v>R&amp;D</v>
       </c>
       <c r="C12" s="12">
-        <v>43950</v>
+        <v>47440</v>
       </c>
       <c r="D12" s="12">
-        <v>45585</v>
+        <v>14469</v>
       </c>
       <c r="E12" s="13">
-        <v>-1635</v>
+        <v>32971</v>
       </c>
       <c r="F12" s="14" t="str">
-        <v>-3.72%</v>
+        <v>69.5%</v>
       </c>
       <c r="G12" s="11" t="str">
         <v/>
@@ -1467,19 +1467,19 @@
         <v/>
       </c>
       <c r="B13" s="17" t="str">
-        <v>Customer Support</v>
+        <v>Human Resources</v>
       </c>
       <c r="C13" s="18">
-        <v>44675</v>
+        <v>62301</v>
       </c>
       <c r="D13" s="18">
-        <v>48472</v>
-      </c>
-      <c r="E13" s="19">
-        <v>-3797</v>
-      </c>
-      <c r="F13" s="20" t="str">
-        <v>-8.5%</v>
+        <v>7768</v>
+      </c>
+      <c r="E13" s="24">
+        <v>54533</v>
+      </c>
+      <c r="F13" s="25" t="str">
+        <v>87.53%</v>
       </c>
       <c r="G13" s="17" t="str">
         <v/>
@@ -1496,34 +1496,34 @@
     </row>
     <row r="14" ht="30" customHeight="1">
       <c r="A14" s="4" t="str">
-        <v>2023-10</v>
+        <v>2023-09</v>
       </c>
       <c r="B14" s="5" t="str">
-        <v>R&amp;D</v>
+        <v>Sales</v>
       </c>
       <c r="C14" s="6">
-        <v>25523</v>
+        <v>69580</v>
       </c>
       <c r="D14" s="6">
-        <v>45948</v>
-      </c>
-      <c r="E14" s="26">
-        <v>-20425</v>
-      </c>
-      <c r="F14" s="27" t="str">
-        <v>-80.03%</v>
+        <v>16886</v>
+      </c>
+      <c r="E14" s="7">
+        <v>52694</v>
+      </c>
+      <c r="F14" s="8" t="str">
+        <v>75.73%</v>
       </c>
       <c r="G14" s="6">
-        <v>95012</v>
+        <v>232648</v>
       </c>
       <c r="H14" s="6">
-        <v>133005</v>
-      </c>
-      <c r="I14" s="26">
-        <v>-37993</v>
-      </c>
-      <c r="J14" s="28">
-        <v>-51.35666666666666</v>
+        <v>83522</v>
+      </c>
+      <c r="I14" s="7">
+        <v>149126</v>
+      </c>
+      <c r="J14" s="9">
+        <v>63.95666666666667</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
@@ -1534,16 +1534,16 @@
         <v>Human Resources</v>
       </c>
       <c r="C15" s="12">
-        <v>43596</v>
+        <v>70895</v>
       </c>
       <c r="D15" s="12">
-        <v>39648</v>
-      </c>
-      <c r="E15" s="22">
-        <v>3948</v>
-      </c>
-      <c r="F15" s="23" t="str">
-        <v>9.06%</v>
+        <v>35495</v>
+      </c>
+      <c r="E15" s="13">
+        <v>35400</v>
+      </c>
+      <c r="F15" s="14" t="str">
+        <v>49.93%</v>
       </c>
       <c r="G15" s="11" t="str">
         <v/>
@@ -1563,19 +1563,19 @@
         <v/>
       </c>
       <c r="B16" s="17" t="str">
-        <v>Marketing</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C16" s="18">
-        <v>25893</v>
+        <v>92173</v>
       </c>
       <c r="D16" s="18">
-        <v>47409</v>
-      </c>
-      <c r="E16" s="19">
-        <v>-21516</v>
-      </c>
-      <c r="F16" s="20" t="str">
-        <v>-83.1%</v>
+        <v>31141</v>
+      </c>
+      <c r="E16" s="24">
+        <v>61032</v>
+      </c>
+      <c r="F16" s="25" t="str">
+        <v>66.21%</v>
       </c>
       <c r="G16" s="17" t="str">
         <v/>
@@ -1592,34 +1592,34 @@
     </row>
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="4" t="str">
-        <v>2023-05</v>
+        <v>2023-09</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Sales</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C17" s="6">
-        <v>12624</v>
+        <v>34994</v>
       </c>
       <c r="D17" s="6">
-        <v>19448</v>
-      </c>
-      <c r="E17" s="26">
-        <v>-6824</v>
-      </c>
-      <c r="F17" s="27" t="str">
-        <v>-54.06%</v>
+        <v>6620</v>
+      </c>
+      <c r="E17" s="7">
+        <v>28374</v>
+      </c>
+      <c r="F17" s="8" t="str">
+        <v>81.08%</v>
       </c>
       <c r="G17" s="6">
-        <v>140847</v>
+        <v>153497</v>
       </c>
       <c r="H17" s="6">
-        <v>71511</v>
+        <v>61087</v>
       </c>
       <c r="I17" s="7">
-        <v>69336</v>
+        <v>92410</v>
       </c>
       <c r="J17" s="9">
-        <v>14.466666666666663</v>
+        <v>48.49</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
@@ -1630,16 +1630,16 @@
         <v>R&amp;D</v>
       </c>
       <c r="C18" s="12">
-        <v>45738</v>
+        <v>36233</v>
       </c>
       <c r="D18" s="12">
-        <v>40478</v>
+        <v>44935</v>
       </c>
       <c r="E18" s="22">
-        <v>5260</v>
+        <v>-8702</v>
       </c>
       <c r="F18" s="23" t="str">
-        <v>11.5%</v>
+        <v>-24.02%</v>
       </c>
       <c r="G18" s="11" t="str">
         <v/>
@@ -1659,19 +1659,19 @@
         <v/>
       </c>
       <c r="B19" s="17" t="str">
-        <v>Customer Support</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C19" s="18">
-        <v>82485</v>
+        <v>82270</v>
       </c>
       <c r="D19" s="18">
-        <v>11585</v>
+        <v>9532</v>
       </c>
       <c r="E19" s="24">
-        <v>70900</v>
+        <v>72738</v>
       </c>
       <c r="F19" s="25" t="str">
-        <v>85.96%</v>
+        <v>88.41%</v>
       </c>
       <c r="G19" s="17" t="str">
         <v/>
@@ -1688,34 +1688,34 @@
     </row>
     <row r="20" ht="30" customHeight="1">
       <c r="A20" s="4" t="str">
-        <v>2023-11</v>
+        <v>2023-06</v>
       </c>
       <c r="B20" s="5" t="str">
-        <v>R&amp;D</v>
+        <v>Human Resources</v>
       </c>
       <c r="C20" s="6">
-        <v>67194</v>
+        <v>97059</v>
       </c>
       <c r="D20" s="6">
-        <v>47962</v>
+        <v>49907</v>
       </c>
       <c r="E20" s="7">
-        <v>19232</v>
+        <v>47152</v>
       </c>
       <c r="F20" s="8" t="str">
-        <v>28.62%</v>
+        <v>48.58%</v>
       </c>
       <c r="G20" s="6">
-        <v>144934</v>
+        <v>220262</v>
       </c>
       <c r="H20" s="6">
-        <v>127651</v>
+        <v>94758</v>
       </c>
       <c r="I20" s="7">
-        <v>17283</v>
-      </c>
-      <c r="J20" s="28">
-        <v>-38.39</v>
+        <v>125504</v>
+      </c>
+      <c r="J20" s="9">
+        <v>42.98666666666666</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
@@ -1723,19 +1723,19 @@
         <v/>
       </c>
       <c r="B21" s="11" t="str">
-        <v>Sales</v>
+        <v>Marketing</v>
       </c>
       <c r="C21" s="12">
-        <v>61108</v>
+        <v>88717</v>
       </c>
       <c r="D21" s="12">
-        <v>30927</v>
-      </c>
-      <c r="E21" s="22">
-        <v>30181</v>
-      </c>
-      <c r="F21" s="23" t="str">
-        <v>49.39%</v>
+        <v>5884</v>
+      </c>
+      <c r="E21" s="13">
+        <v>82833</v>
+      </c>
+      <c r="F21" s="14" t="str">
+        <v>93.37%</v>
       </c>
       <c r="G21" s="11" t="str">
         <v/>
@@ -1758,16 +1758,16 @@
         <v>Sales</v>
       </c>
       <c r="C22" s="18">
-        <v>16632</v>
+        <v>34486</v>
       </c>
       <c r="D22" s="18">
-        <v>48762</v>
+        <v>38967</v>
       </c>
       <c r="E22" s="19">
-        <v>-32130</v>
+        <v>-4481</v>
       </c>
       <c r="F22" s="20" t="str">
-        <v>-193.18%</v>
+        <v>-12.99%</v>
       </c>
       <c r="G22" s="17" t="str">
         <v/>
@@ -1784,34 +1784,34 @@
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="4" t="str">
-        <v>2023-10</v>
+        <v>2023-12</v>
       </c>
       <c r="B23" s="5" t="str">
         <v>Marketing</v>
       </c>
       <c r="C23" s="6">
-        <v>81697</v>
+        <v>84827</v>
       </c>
       <c r="D23" s="6">
-        <v>28754</v>
+        <v>46709</v>
       </c>
       <c r="E23" s="7">
-        <v>52943</v>
+        <v>38118</v>
       </c>
       <c r="F23" s="8" t="str">
-        <v>64.8%</v>
+        <v>44.94%</v>
       </c>
       <c r="G23" s="6">
-        <v>209145</v>
+        <v>203207</v>
       </c>
       <c r="H23" s="6">
-        <v>104697</v>
+        <v>109645</v>
       </c>
       <c r="I23" s="7">
-        <v>104448</v>
+        <v>93562</v>
       </c>
       <c r="J23" s="9">
-        <v>36.21333333333333</v>
+        <v>26.52333333333333</v>
       </c>
     </row>
     <row r="24" ht="30" customHeight="1">
@@ -1819,19 +1819,19 @@
         <v/>
       </c>
       <c r="B24" s="11" t="str">
-        <v>R&amp;D</v>
+        <v>Customer Support</v>
       </c>
       <c r="C24" s="12">
-        <v>98040</v>
+        <v>25011</v>
       </c>
       <c r="D24" s="12">
-        <v>42882</v>
+        <v>33468</v>
       </c>
       <c r="E24" s="22">
-        <v>55158</v>
+        <v>-8457</v>
       </c>
       <c r="F24" s="23" t="str">
-        <v>56.26%</v>
+        <v>-33.81%</v>
       </c>
       <c r="G24" s="11" t="str">
         <v/>
@@ -1851,19 +1851,19 @@
         <v/>
       </c>
       <c r="B25" s="17" t="str">
-        <v>Sales</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C25" s="18">
-        <v>29408</v>
+        <v>93369</v>
       </c>
       <c r="D25" s="18">
-        <v>33061</v>
-      </c>
-      <c r="E25" s="19">
-        <v>-3653</v>
-      </c>
-      <c r="F25" s="20" t="str">
-        <v>-12.42%</v>
+        <v>29468</v>
+      </c>
+      <c r="E25" s="24">
+        <v>63901</v>
+      </c>
+      <c r="F25" s="25" t="str">
+        <v>68.44%</v>
       </c>
       <c r="G25" s="17" t="str">
         <v/>
@@ -1880,34 +1880,34 @@
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="A26" s="4" t="str">
-        <v>2023-09</v>
+        <v>2023-10</v>
       </c>
       <c r="B26" s="5" t="str">
-        <v>R&amp;D</v>
+        <v>Customer Support</v>
       </c>
       <c r="C26" s="6">
-        <v>53606</v>
+        <v>13238</v>
       </c>
       <c r="D26" s="6">
-        <v>6800</v>
-      </c>
-      <c r="E26" s="7">
-        <v>46806</v>
-      </c>
-      <c r="F26" s="8" t="str">
-        <v>87.31%</v>
+        <v>37861</v>
+      </c>
+      <c r="E26" s="26">
+        <v>-24623</v>
+      </c>
+      <c r="F26" s="27" t="str">
+        <v>-186%</v>
       </c>
       <c r="G26" s="6">
-        <v>159235</v>
+        <v>38168</v>
       </c>
       <c r="H26" s="6">
-        <v>66799</v>
-      </c>
-      <c r="I26" s="7">
-        <v>92436</v>
-      </c>
-      <c r="J26" s="9">
-        <v>58.553333333333335</v>
+        <v>115363</v>
+      </c>
+      <c r="I26" s="26">
+        <v>-77195</v>
+      </c>
+      <c r="J26" s="28">
+        <v>-207.06000000000003</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1">
@@ -1918,16 +1918,16 @@
         <v>Marketing</v>
       </c>
       <c r="C27" s="12">
-        <v>56996</v>
+        <v>14532</v>
       </c>
       <c r="D27" s="12">
-        <v>38845</v>
+        <v>40271</v>
       </c>
       <c r="E27" s="22">
-        <v>18151</v>
+        <v>-25739</v>
       </c>
       <c r="F27" s="23" t="str">
-        <v>31.85%</v>
+        <v>-177.12%</v>
       </c>
       <c r="G27" s="11" t="str">
         <v/>
@@ -1950,16 +1950,16 @@
         <v>Customer Support</v>
       </c>
       <c r="C28" s="18">
-        <v>48633</v>
+        <v>10398</v>
       </c>
       <c r="D28" s="18">
-        <v>21154</v>
-      </c>
-      <c r="E28" s="24">
-        <v>27479</v>
-      </c>
-      <c r="F28" s="25" t="str">
-        <v>56.5%</v>
+        <v>37231</v>
+      </c>
+      <c r="E28" s="19">
+        <v>-26833</v>
+      </c>
+      <c r="F28" s="20" t="str">
+        <v>-258.06%</v>
       </c>
       <c r="G28" s="17" t="str">
         <v/>
@@ -1976,34 +1976,34 @@
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" s="4" t="str">
-        <v>2023-11</v>
+        <v>2023-05</v>
       </c>
       <c r="B29" s="5" t="str">
         <v>Customer Support</v>
       </c>
       <c r="C29" s="6">
-        <v>48056</v>
+        <v>84822</v>
       </c>
       <c r="D29" s="6">
-        <v>30383</v>
+        <v>28335</v>
       </c>
       <c r="E29" s="7">
-        <v>17673</v>
+        <v>56487</v>
       </c>
       <c r="F29" s="8" t="str">
-        <v>36.78%</v>
+        <v>66.59%</v>
       </c>
       <c r="G29" s="6">
-        <v>138701</v>
+        <v>154584</v>
       </c>
       <c r="H29" s="6">
-        <v>69900</v>
+        <v>84333</v>
       </c>
       <c r="I29" s="7">
-        <v>68801</v>
+        <v>70251</v>
       </c>
       <c r="J29" s="9">
-        <v>45.126666666666665</v>
+        <v>37.11333333333334</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1">
@@ -2011,19 +2011,19 @@
         <v/>
       </c>
       <c r="B30" s="11" t="str">
-        <v>Marketing</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C30" s="12">
-        <v>57529</v>
+        <v>40004</v>
       </c>
       <c r="D30" s="12">
-        <v>13987</v>
-      </c>
-      <c r="E30" s="22">
-        <v>43542</v>
-      </c>
-      <c r="F30" s="23" t="str">
-        <v>75.69%</v>
+        <v>38266</v>
+      </c>
+      <c r="E30" s="13">
+        <v>1738</v>
+      </c>
+      <c r="F30" s="14" t="str">
+        <v>4.34%</v>
       </c>
       <c r="G30" s="11" t="str">
         <v/>
@@ -2046,16 +2046,16 @@
         <v>Human Resources</v>
       </c>
       <c r="C31" s="18">
-        <v>33116</v>
+        <v>29758</v>
       </c>
       <c r="D31" s="18">
-        <v>25530</v>
+        <v>17732</v>
       </c>
       <c r="E31" s="24">
-        <v>7586</v>
+        <v>12026</v>
       </c>
       <c r="F31" s="25" t="str">
-        <v>22.91%</v>
+        <v>40.41%</v>
       </c>
       <c r="G31" s="17" t="str">
         <v/>
@@ -2072,16 +2072,16 @@
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="G32" s="29">
-        <v>1592808</v>
+        <v>1706015</v>
       </c>
       <c r="H32" s="29">
-        <v>1046492</v>
+        <v>887654</v>
       </c>
       <c r="I32" s="30">
-        <v>546316</v>
+        <v>818361</v>
       </c>
       <c r="J32" s="31">
-        <v>15.261333333333335</v>
+        <v>17.074666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>